<commit_message>
Videoloeng 3; 28:40 peal
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906F331F-4F98-4C66-94D0-489EF1B23652}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A12FAC-E33D-4F0B-BA1C-3CC438F7269A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19692" windowHeight="11928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>tekkisid namespace-i vead CRUD lehekülgedel</t>
+  </si>
+  <si>
+    <t>Videoloeng 3</t>
   </si>
 </sst>
 </file>
@@ -2870,7 +2873,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3130,14 +3133,18 @@
         <v>6</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7">
+        <v>0.53611111111111109</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5"/>
       <c r="F12" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>-772</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
@@ -3332,7 +3339,7 @@
       <c r="E23" s="36"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>403</v>
+        <v>-369</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL3; 1.03 + logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB508C4-ED49-4DB1-BD40-C85AF547D164}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F78AF43-D33B-49FE-B14A-9ABB373761A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19692" windowHeight="11928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="67">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -239,6 +239,9 @@
   </si>
   <si>
     <t>Videoloeng 3</t>
+  </si>
+  <si>
+    <t>Videoloeng 3 jätk</t>
   </si>
 </sst>
 </file>
@@ -2873,7 +2876,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3158,15 +3161,21 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="6">
+        <v>43882</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.42569444444444443</v>
+      </c>
       <c r="D13" s="7"/>
       <c r="E13" s="5"/>
       <c r="F13" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>-613</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
@@ -3343,7 +3352,7 @@
       <c r="E23" s="36"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>517.00000000000011</v>
+        <v>-95.999999999999886</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
vl3 lõpuni; index.cshtml foreach tsükkel annab nullref.exceptioni rakenduse käivitamisel. +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F78AF43-D33B-49FE-B14A-9ABB373761A0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B19D8E1-BC50-4E21-9F36-A02151C07285}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19692" windowHeight="11928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="68">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>Videoloeng 3 jätk</t>
+  </si>
+  <si>
+    <t>nullref.exception index.cshtml faili foreach tsüklis</t>
   </si>
 </sst>
 </file>
@@ -2875,7 +2878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB595BE-6E2E-4B1E-A535-41207EE689C5}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -3167,16 +3170,22 @@
       <c r="C13" s="7">
         <v>0.42569444444444443</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="7">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
       <c r="F13" s="30">
         <f t="shared" si="0"/>
-        <v>-613</v>
+        <v>111</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
@@ -3352,7 +3361,7 @@
       <c r="E23" s="36"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>-95.999999999999886</v>
+        <v>628.00000000000011</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL4, 2 helper meetodit nullref.excep index lehel ikka +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B19D8E1-BC50-4E21-9F36-A02151C07285}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9F1F13-437F-46C8-B5C7-D15EFEB7F341}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19692" windowHeight="11928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="71">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>nullref.exception index.cshtml faili foreach tsüklis</t>
+  </si>
+  <si>
+    <t>Videoloeng 4</t>
+  </si>
+  <si>
+    <t>Videoloeng 4 jätk</t>
+  </si>
+  <si>
+    <t>nullref.exception index.cshtml faili foreach tsüklis ikka sees</t>
   </si>
 </sst>
 </file>
@@ -2878,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB595BE-6E2E-4B1E-A535-41207EE689C5}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3186,7 +3195,9 @@
       <c r="H13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3195,14 +3206,22 @@
         <v>8</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="7">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.6958333333333333</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
       <c r="F14" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="5"/>
+        <v>51.999999999999972</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
@@ -3213,16 +3232,28 @@
         <v>9</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="7">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.75555555555555554</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
       <c r="F15" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+        <v>38.000000000000028</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3361,7 +3392,7 @@
       <c r="E23" s="36"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>628.00000000000011</v>
+        <v>718.00000000000011</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL5; nullref exceptionist sain lahti; tuli uus: InvalidCastException: Unable to cast object of type 'System.Collections.Generic.List`1[System.Object]' to type 'Microsoft.AspNetCore.Html.IHtmlContent'.
+logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9F1F13-437F-46C8-B5C7-D15EFEB7F341}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643F607D-381A-4A41-B43F-C2E0B5D28224}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19692" windowHeight="11928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="73">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>nullref.exception index.cshtml faili foreach tsüklis ikka sees</t>
+  </si>
+  <si>
+    <t>Videoloeng 5</t>
+  </si>
+  <si>
+    <t>nullref ex läks korda, uued exceptionid selle asemel: InvalidCastException: Unable to cast object of type 'System.Collections.Generic.List`1[System.Object]' to type 'Microsoft.AspNetCore.Html.IHtmlContent'.</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -713,6 +719,30 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2888,7 +2918,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2900,7 +2930,7 @@
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" customWidth="1"/>
     <col min="7" max="7" width="55.77734375" customWidth="1"/>
-    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="8" max="8" width="72.109375" customWidth="1"/>
     <col min="9" max="9" width="3.44140625" customWidth="1"/>
     <col min="10" max="10" width="8.6640625" customWidth="1"/>
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
@@ -3256,23 +3286,37 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+    <row r="16" spans="1:14" s="58" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="51">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="8"/>
+      <c r="B16" s="52">
+        <v>43883</v>
+      </c>
+      <c r="C16" s="53">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="D16" s="53">
+        <v>0.82986111111111116</v>
+      </c>
+      <c r="E16" s="54">
+        <v>0</v>
+      </c>
+      <c r="F16" s="55">
+        <f t="shared" si="0"/>
+        <v>50.000000000000142</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
@@ -3392,7 +3436,7 @@
       <c r="E23" s="36"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>718.00000000000011</v>
+        <v>768.00000000000023</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
@@ -3410,7 +3454,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Search lahtri-buttoni lsiamine; exception ikka olemas; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643F607D-381A-4A41-B43F-C2E0B5D28224}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82424817-69AA-4874-AE74-2B34E197C937}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19692" windowHeight="11928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="77">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -260,6 +260,18 @@
   </si>
   <si>
     <t>nullref ex läks korda, uued exceptionid selle asemel: InvalidCastException: Unable to cast object of type 'System.Collections.Generic.List`1[System.Object]' to type 'Microsoft.AspNetCore.Html.IHtmlContent'.</t>
+  </si>
+  <si>
+    <t>Videoloeng 6</t>
+  </si>
+  <si>
+    <t>sama exception ikka alles, mis enne; search buttoni asemel genereeris textboxi, milles kirjas Search</t>
+  </si>
+  <si>
+    <t>Vigade parandus</t>
+  </si>
+  <si>
+    <t>search buttoni sain korda, exception ikka olemas</t>
   </si>
 </sst>
 </file>
@@ -612,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -663,6 +675,30 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -720,29 +756,61 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,68 +1149,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="52">
         <v>43863</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1624,13 +1692,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0.71180555555555591</v>
@@ -1680,68 +1748,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="52">
         <v>43871</v>
       </c>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2329,13 +2397,13 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="36"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
       <c r="F27" s="25">
         <f>SUM(F7:F26)</f>
         <v>0.77291666666666681</v>
@@ -2385,66 +2453,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2882,13 +2950,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>1260.0000000000002</v>
@@ -2918,7 +2986,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2930,7 +2998,7 @@
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" customWidth="1"/>
     <col min="7" max="7" width="55.77734375" customWidth="1"/>
-    <col min="8" max="8" width="72.109375" customWidth="1"/>
+    <col min="8" max="8" width="72.109375" style="39" customWidth="1"/>
     <col min="9" max="9" width="3.44140625" customWidth="1"/>
     <col min="10" max="10" width="8.6640625" customWidth="1"/>
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
@@ -2938,66 +3006,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="A2" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="64"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="67"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="69"/>
+      <c r="C4" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="72"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="75"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3046,7 +3114,7 @@
       <c r="G7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="17"/>
+      <c r="H7" s="82"/>
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
       <c r="N7" t="s">
@@ -3075,7 +3143,7 @@
       <c r="G8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="35" t="s">
         <v>61</v>
       </c>
       <c r="I8" s="5"/>
@@ -3108,7 +3176,7 @@
       <c r="G9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="35"/>
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
@@ -3134,7 +3202,7 @@
       <c r="G10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="35"/>
       <c r="I10" s="5" t="s">
         <v>14</v>
       </c>
@@ -3164,7 +3232,7 @@
       <c r="G11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="35" t="s">
         <v>64</v>
       </c>
       <c r="I11" s="5" t="s">
@@ -3194,7 +3262,7 @@
       <c r="G12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="35"/>
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
@@ -3222,7 +3290,7 @@
       <c r="G13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="35" t="s">
         <v>67</v>
       </c>
       <c r="I13" s="5" t="s">
@@ -3252,7 +3320,7 @@
       <c r="G14" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="35"/>
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
@@ -3278,7 +3346,7 @@
       <c r="G15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="35" t="s">
         <v>70</v>
       </c>
       <c r="I15" s="5" t="s">
@@ -3286,53 +3354,65 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" s="58" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="51">
+    <row r="16" spans="1:14" s="39" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="32">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B16" s="52">
+      <c r="B16" s="33">
         <v>43883</v>
       </c>
-      <c r="C16" s="53">
+      <c r="C16" s="34">
         <v>0.79513888888888884</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="34">
         <v>0.82986111111111116</v>
       </c>
-      <c r="E16" s="54">
-        <v>0</v>
-      </c>
-      <c r="F16" s="55">
+      <c r="E16" s="35">
+        <v>0</v>
+      </c>
+      <c r="F16" s="36">
         <f t="shared" si="0"/>
         <v>50.000000000000142</v>
       </c>
-      <c r="G16" s="54" t="s">
+      <c r="G16" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="56" t="s">
+      <c r="H16" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="57"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="5"/>
+      <c r="B17" s="6">
+        <v>43884</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.56319444444444444</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
       <c r="F17" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+        <v>35.000000000000036</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
@@ -3342,15 +3422,25 @@
         <v>12</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
+      <c r="C18" s="7">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.59583333333333333</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
       <c r="F18" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+        <v>10.999999999999961</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>76</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
@@ -3368,7 +3458,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="35"/>
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
@@ -3386,7 +3476,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="H20" s="35"/>
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
@@ -3404,7 +3494,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="35"/>
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
@@ -3422,37 +3512,28 @@
         <v>0</v>
       </c>
       <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="H22" s="83"/>
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>768.00000000000023</v>
+        <v>814.00000000000023</v>
       </c>
       <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="H23" s="84"/>
       <c r="I23" s="23"/>
       <c r="J23" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A2:J3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:B6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -3483,66 +3564,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="A2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="47"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="58"/>
+      <c r="C4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="53"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="48"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="56"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="33"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3819,13 +3900,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0</v>

</xml_diff>

<commit_message>
MEasures(CRUD) ja extensions uuesti
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B366ABE-3A5E-4061-B471-A6E340A9FFBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDD9FEC-0D3D-4BA2-9005-702FB539B9D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="77">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -756,67 +756,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1155,68 +1155,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="77" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="78">
+      <c r="G4" s="81">
         <v>43863</v>
       </c>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="82"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="67"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1698,13 +1698,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0.71180555555555591</v>
@@ -1754,68 +1754,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="77" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="78">
+      <c r="G4" s="81">
         <v>43871</v>
       </c>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="82"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="67"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2403,13 +2403,13 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="70"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="73"/>
       <c r="F27" s="25">
         <f>SUM(F7:F26)</f>
         <v>0.77291666666666681</v>
@@ -2459,66 +2459,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="77" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="82"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="67"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2956,13 +2956,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>1260.0000000000002</v>
@@ -3550,7 +3550,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3560,7 +3560,7 @@
     <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11" style="85" customWidth="1"/>
+    <col min="6" max="6" width="11" style="66" customWidth="1"/>
     <col min="7" max="7" width="55.77734375" customWidth="1"/>
     <col min="8" max="8" width="63.44140625" customWidth="1"/>
     <col min="9" max="9" width="3.44140625" customWidth="1"/>
@@ -3570,66 +3570,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="77" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="86" t="s">
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="82"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="67"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3639,7 +3639,7 @@
       <c r="E6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="68" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -3690,15 +3690,21 @@
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="6">
+        <v>43888</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="D8" s="7"/>
       <c r="E8" s="5"/>
       <c r="F8" s="30">
         <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>-480</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="8"/>
@@ -3959,16 +3965,16 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>90</v>
+        <v>-390</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
@@ -4015,66 +4021,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="74"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="77" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="80"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="82"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="67"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4351,13 +4357,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0</v>

</xml_diff>

<commit_message>
VL7; andmebaasi, migratsioonide uuendused; logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDD9FEC-0D3D-4BA2-9005-702FB539B9D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A6D4C-36ED-4043-B6EC-FBD36AFECB94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="78">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>search buttoni sain korda, exception ikka olemas</t>
+  </si>
+  <si>
+    <t>eelmised parandused + VL7</t>
   </si>
 </sst>
 </file>
@@ -3550,7 +3553,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3696,16 +3699,22 @@
       <c r="C8" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="7">
+        <v>0.43888888888888888</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
       <c r="F8" s="30">
         <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
-        <v>-480</v>
+        <v>152.00000000000003</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="8"/>
       <c r="N8" t="s">
@@ -3974,7 +3983,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>-390</v>
+        <v>242.00000000000003</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL10 - testide baasklassid; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E8A436-32E9-4F31-A1A1-9E320D5AB6F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE8FD08-4D99-45BA-9BEF-06CF2CF6B290}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -282,6 +282,15 @@
   </si>
   <si>
     <t>eelmised parandused + VL7 (kodutöö 5)</t>
+  </si>
+  <si>
+    <t>Videoloeng 10</t>
+  </si>
+  <si>
+    <t>Testimise alustamine</t>
+  </si>
+  <si>
+    <t>Testimise baasklassid</t>
   </si>
 </sst>
 </file>
@@ -3558,8 +3567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3775,7 +3784,9 @@
       <c r="G10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
@@ -3785,15 +3796,25 @@
         <v>5</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="7">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.7090277777777777</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
       <c r="F11" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+        <v>134.99999999999983</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
@@ -4005,7 +4026,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>356.00000000000011</v>
+        <v>490.99999999999994</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL11 poole peal: "unknown project"'i all 2 testi - tekkis unknown error rebuildimisel; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE8FD08-4D99-45BA-9BEF-06CF2CF6B290}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2A572D-82EB-4E00-B119-393BA57C339F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="85">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>Testimise baasklassid</t>
+  </si>
+  <si>
+    <t>Videoloeng 11</t>
+  </si>
+  <si>
+    <t>Pooleli 17:48 peal; Atribuutide testimine; 2 testi läksid "Unknown project"i alla ja neid ei tunta ära - error.</t>
   </si>
 </sst>
 </file>
@@ -3567,8 +3573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D4" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3580,7 +3586,7 @@
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="11" style="66" customWidth="1"/>
     <col min="7" max="7" width="55.77734375" customWidth="1"/>
-    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="8" max="8" width="92.88671875" customWidth="1"/>
     <col min="9" max="9" width="3.44140625" customWidth="1"/>
     <col min="10" max="10" width="8.6640625" customWidth="1"/>
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
@@ -3730,7 +3736,9 @@
       <c r="H8" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J8" s="8"/>
       <c r="N8" t="s">
         <v>15</v>
@@ -3759,7 +3767,9 @@
         <v>77</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3787,7 +3797,9 @@
       <c r="H10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3815,7 +3827,9 @@
       <c r="H11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3824,15 +3838,25 @@
         <v>6</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="7">
+        <v>0.73055555555555562</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.75416666666666676</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
       <c r="F12" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+        <v>34.000000000000043</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
@@ -4026,7 +4050,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>490.99999999999994</v>
+        <v>525</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL11 - kood peale testide lõppu +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF792CA-D2CC-4FA4-95B6-6BD71F747DC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96F61CF-9324-4CB8-88D4-B9D4DE0B340A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3576,8 +3576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3874,11 +3874,15 @@
       <c r="C13" s="7">
         <v>0.60416666666666663</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="7">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
       <c r="F13" s="30">
         <f t="shared" si="0"/>
-        <v>-870</v>
+        <v>45</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>85</v>
@@ -4059,7 +4063,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>-345</v>
+        <v>570</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL12 - Repositooriumite refaktoorimine; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96F61CF-9324-4CB8-88D4-B9D4DE0B340A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C96B21E-126F-4D59-955D-39E9B2CC9566}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="88">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>Videoloeng 11 jätk</t>
+  </si>
+  <si>
+    <t>Videoloeng 12</t>
+  </si>
+  <si>
+    <t>Reporitooriumite refaktoorimine</t>
   </si>
 </sst>
 </file>
@@ -3576,8 +3582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3888,7 +3894,9 @@
         <v>85</v>
       </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3897,15 +3905,25 @@
         <v>8</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="7">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
       <c r="F14" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+        <v>41.000000000000014</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
@@ -4063,7 +4081,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>570</v>
+        <v>611</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL  12 lõpuni; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C96B21E-126F-4D59-955D-39E9B2CC9566}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA2B17E-7D70-4365-B9AD-96EB537019E4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="89">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -306,6 +306,9 @@
   </si>
   <si>
     <t>Reporitooriumite refaktoorimine</t>
+  </si>
+  <si>
+    <t>Videolong 12 jätk</t>
   </si>
 </sst>
 </file>
@@ -3583,7 +3586,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3933,14 +3936,22 @@
         <v>9</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="7">
+        <v>0.71875</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
       <c r="F15" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="5"/>
+        <v>25.000000000000071</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
@@ -4081,7 +4092,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>611</v>
+        <v>636.00000000000011</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL15 - vaadete mallid (template); +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E007B1-8F55-45FC-A455-52A700D069B5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002FC925-BAB0-402D-A731-971895484A9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="97">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -327,6 +327,12 @@
   </si>
   <si>
     <t>Kood baseRepository klassis</t>
+  </si>
+  <si>
+    <t>Videoloeng 15</t>
+  </si>
+  <si>
+    <t>Vaadete mallid (template)</t>
   </si>
 </sst>
 </file>
@@ -679,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -871,6 +877,15 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3601,10 +3616,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3757,7 +3772,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="30">
-        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+        <f t="shared" ref="F8:F27" si="0">(D8-C8)*1440</f>
         <v>152.00000000000003</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -3776,7 +3791,7 @@
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
-        <f t="shared" ref="A9:A22" si="1">A8+1</f>
+        <f t="shared" ref="A9:A20" si="1">A8+1</f>
         <v>3</v>
       </c>
       <c r="B9" s="6"/>
@@ -4098,21 +4113,32 @@
         <v>14</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
+      <c r="C20" s="7">
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.95416666666666661</v>
+      </c>
+      <c r="E20" s="5">
+        <v>5</v>
+      </c>
       <c r="F20" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+        <v>61.999999999999943</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
-        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B21" s="6"/>
@@ -4130,42 +4156,126 @@
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
-        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="14">
+        <v>17</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="14">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14">
+        <v>19</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14">
+        <v>20</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="14">
         <v>21</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="31">
-        <f>SUM(F7:F22)</f>
-        <v>805.00000000000057</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="22"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="89"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="31">
+        <f>SUM(F7:F27)</f>
+        <v>867.00000000000045</v>
+      </c>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A28:E28"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>

<commit_message>
VL16 - template jätk, +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002FC925-BAB0-402D-A731-971895484A9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3063356A-2CAE-4C65-8821-2D9B43AFE694}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="99">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -333,6 +333,12 @@
   </si>
   <si>
     <t>Vaadete mallid (template)</t>
+  </si>
+  <si>
+    <t>Videoloeng 16</t>
+  </si>
+  <si>
+    <t>template jätk</t>
   </si>
 </sst>
 </file>
@@ -3619,7 +3625,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4142,16 +4148,28 @@
         <v>15</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="7">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.4201388888888889</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
       <c r="F21" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+        <v>78.000000000000043</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4266,7 +4284,7 @@
       <c r="E28" s="90"/>
       <c r="F28" s="31">
         <f>SUM(F7:F27)</f>
-        <v>867.00000000000045</v>
+        <v>945.00000000000045</v>
       </c>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>

</xml_diff>

<commit_message>
VL17 - template lõpp; sortimine; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71A3481-AB31-4F27-BD96-4492D7EF661D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD5C863-BE99-44CE-9985-565F2E736716}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="102">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>template jätk; extension failid…</t>
+  </si>
+  <si>
+    <t>template lõpp</t>
   </si>
 </sst>
 </file>
@@ -3631,7 +3634,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4210,16 +4213,28 @@
         <v>17</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="5"/>
+      <c r="C23" s="7">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0.54097222222222219</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
       <c r="F23" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+        <v>95.999999999999972</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4300,7 +4315,7 @@
       <c r="E28" s="90"/>
       <c r="F28" s="31">
         <f>SUM(F7:F27)</f>
-        <v>962.00000000000034</v>
+        <v>1058.0000000000002</v>
       </c>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>

</xml_diff>

<commit_message>
VL 18; SortedRepository abstraktseks; VL 19; SortedRepository vigade parandus; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD5C863-BE99-44CE-9985-565F2E736716}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610FD6A-18ED-4F5E-8A68-8949DFDAB748}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Nädal 3" sheetId="5" r:id="rId3"/>
     <sheet name="Nädal 4" sheetId="6" r:id="rId4"/>
     <sheet name="Nädal5" sheetId="7" r:id="rId5"/>
-    <sheet name="Nädal" sheetId="4" r:id="rId6"/>
+    <sheet name="Nädal6" sheetId="8" r:id="rId6"/>
+    <sheet name="Nädal" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="107">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -348,6 +349,21 @@
   </si>
   <si>
     <t>template lõpp</t>
+  </si>
+  <si>
+    <t>Total Time (min) :</t>
+  </si>
+  <si>
+    <t>VL 18</t>
+  </si>
+  <si>
+    <t>SortedRepository akstraktseks</t>
+  </si>
+  <si>
+    <t>VL 19</t>
+  </si>
+  <si>
+    <t>SortedRepository akstraktseks parandused</t>
   </si>
 </sst>
 </file>
@@ -3633,7 +3649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -4338,11 +4354,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD61791-7BB1-422F-B003-B0D8AC44CC15}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4352,7 +4368,7 @@
     <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11" style="66" customWidth="1"/>
     <col min="7" max="7" width="55.77734375" customWidth="1"/>
     <col min="8" max="8" width="63.44140625" customWidth="1"/>
     <col min="9" max="9" width="3.44140625" customWidth="1"/>
@@ -4397,7 +4413,7 @@
       </c>
       <c r="D4" s="80"/>
       <c r="E4" s="80"/>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="81"/>
@@ -4431,7 +4447,468 @@
       <c r="E6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
+      <c r="B7" s="15">
+        <v>43892</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.68194444444444446</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
+        <f>(D7-C7)*1440</f>
+        <v>70.000000000000071</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14">
+        <f>A7+1</f>
+        <v>2</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7">
+        <v>0.68263888888888891</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="30">
+        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+        <v>17.000000000000099</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="8"/>
+      <c r="N8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14">
+        <f t="shared" ref="A9:A22" si="1">A8+1</f>
+        <v>3</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="14">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="31">
+        <f>SUM(F7:F22)</f>
+        <v>87.000000000000171</v>
+      </c>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11" style="66" customWidth="1"/>
+    <col min="7" max="7" width="55.77734375" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="79"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="87"/>
+      <c r="C4" s="80" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="82"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="85"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="70"/>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="68" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -4457,8 +4934,8 @@
       <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7" s="16">
-        <f>D7-C7</f>
+      <c r="F7" s="30">
+        <f>(D7-C7)*1440</f>
         <v>0</v>
       </c>
       <c r="G7" s="17"/>
@@ -4478,7 +4955,10 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="16"/>
+      <c r="F8" s="30">
+        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+        <v>0</v>
+      </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -4489,14 +4969,17 @@
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
-        <f t="shared" ref="A9:A22" si="0">A8+1</f>
+        <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="16"/>
+      <c r="F9" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -4504,14 +4987,17 @@
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="16"/>
+      <c r="F10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -4519,14 +5005,17 @@
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="16"/>
+      <c r="F11" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -4534,14 +5023,17 @@
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="16"/>
+      <c r="F12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -4549,14 +5041,17 @@
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="16"/>
+      <c r="F13" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -4564,14 +5059,17 @@
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="16"/>
+      <c r="F14" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -4579,14 +5077,17 @@
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="16"/>
+      <c r="F15" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -4594,14 +5095,17 @@
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="16"/>
+      <c r="F16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -4609,14 +5113,17 @@
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="16"/>
+      <c r="F17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -4624,14 +5131,17 @@
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="16"/>
+      <c r="F18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -4639,14 +5149,17 @@
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="16"/>
+      <c r="F19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -4654,14 +5167,17 @@
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="16"/>
+      <c r="F20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -4669,14 +5185,17 @@
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="16"/>
+      <c r="F21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -4684,14 +5203,17 @@
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="21"/>
-      <c r="F22" s="16"/>
+      <c r="F22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
@@ -4699,13 +5221,13 @@
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="71" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="B23" s="72"/>
       <c r="C23" s="72"/>
       <c r="D23" s="72"/>
       <c r="E23" s="73"/>
-      <c r="F23" s="25">
+      <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
VL20; SortedRepository testid I; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2610FD6A-18ED-4F5E-8A68-8949DFDAB748}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AAB8EE-3E00-418F-8E62-8482505743E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="1032" windowWidth="11436" windowHeight="11928" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="109">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>SortedRepository akstraktseks parandused</t>
+  </si>
+  <si>
+    <t>VL20</t>
+  </si>
+  <si>
+    <t>SortedRepository testid</t>
   </si>
 </sst>
 </file>
@@ -4357,8 +4363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD61791-7BB1-422F-B003-B0D8AC44CC15}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4535,17 +4541,31 @@
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="6">
+        <v>43893</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
       <c r="F9" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+        <v>53.000000000000128</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4792,7 +4812,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>87.000000000000171</v>
+        <v>140.00000000000028</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL21 - sortedRepository testid2; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AAB8EE-3E00-418F-8E62-8482505743E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B91F532-D4C9-49FE-A38F-2A6342E57ECA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="111">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -370,6 +370,12 @@
   </si>
   <si>
     <t>SortedRepository testid</t>
+  </si>
+  <si>
+    <t>VL 21</t>
+  </si>
+  <si>
+    <t>SortedRepository testid 2; edit.cshtml annab exceptioni</t>
   </si>
 </sst>
 </file>
@@ -3655,8 +3661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4361,10 +4367,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD61791-7BB1-422F-B003-B0D8AC44CC15}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4519,7 +4525,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="30">
-        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+        <f t="shared" ref="F8:F23" si="0">(D8-C8)*1440</f>
         <v>17.000000000000099</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -4537,77 +4543,93 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
-        <f t="shared" ref="A9:A22" si="1">A8+1</f>
-        <v>3</v>
-      </c>
+      <c r="A9" s="14"/>
       <c r="B9" s="6">
         <v>43893</v>
       </c>
       <c r="C9" s="7">
-        <v>0.64236111111111105</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D9" s="7">
-        <v>0.6791666666666667</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
       <c r="F9" s="30">
         <f t="shared" si="0"/>
-        <v>53.000000000000128</v>
+        <v>90</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
+        <f>A8+1</f>
+        <v>3</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
       <c r="F10" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+        <v>53.000000000000128</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f t="shared" ref="A11:A23" si="1">A10+1</f>
+        <v>4</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="7">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.8881944444444444</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
       <c r="F11" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+        <v>53.999999999999808</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
@@ -4625,7 +4647,7 @@
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
@@ -4643,7 +4665,7 @@
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
@@ -4661,7 +4683,7 @@
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -4679,7 +4701,7 @@
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -4697,7 +4719,7 @@
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -4715,7 +4737,7 @@
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -4733,7 +4755,7 @@
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -4751,7 +4773,7 @@
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -4769,7 +4791,7 @@
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -4787,41 +4809,59 @@
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="14">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="31">
-        <f>SUM(F7:F22)</f>
-        <v>140.00000000000028</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="31">
+        <f>SUM(F7:F23)</f>
+        <v>284.00000000000011</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>

<commit_message>
VL27- lambda expressions; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E824E9EC-7C88-43B9-B688-51602A78CB34}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50B11CE-392B-4E51-8F72-43407600F53A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="24" windowWidth="15588" windowHeight="11928" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6672" yWindow="0" windowWidth="15588" windowHeight="11928" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="130">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -424,6 +424,15 @@
   </si>
   <si>
     <t>FilteredRepository universaalseks</t>
+  </si>
+  <si>
+    <t>VL27</t>
+  </si>
+  <si>
+    <t>LambdaExpression</t>
+  </si>
+  <si>
+    <t>Clean Code</t>
   </si>
 </sst>
 </file>
@@ -4415,10 +4424,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD61791-7BB1-422F-B003-B0D8AC44CC15}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4559,7 +4568,6 @@
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14">
-        <f>A7+1</f>
         <v>2</v>
       </c>
       <c r="B8" s="6"/>
@@ -4573,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="30">
-        <f t="shared" ref="F8:F23" si="0">(D8-C8)*1440</f>
+        <f t="shared" ref="F8:F26" si="0">(D8-C8)*1440</f>
         <v>17.000000000000099</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -4591,7 +4599,9 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14">
+        <v>3</v>
+      </c>
       <c r="B9" s="6">
         <v>43893</v>
       </c>
@@ -4617,8 +4627,7 @@
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14">
-        <f>A8+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="7">
         <v>0.64236111111111105</v>
@@ -4646,8 +4655,7 @@
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14">
-        <f t="shared" ref="A11:A23" si="1">A10+1</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7">
@@ -4676,8 +4684,7 @@
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="14">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="6">
         <v>43894</v>
@@ -4708,8 +4715,7 @@
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7">
@@ -4736,8 +4742,7 @@
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7">
@@ -4762,8 +4767,7 @@
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7">
@@ -4790,230 +4794,309 @@
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B16" s="6">
-        <v>43895</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B16" s="6"/>
       <c r="C16" s="7">
-        <v>0.3972222222222222</v>
+        <v>0.95486111111111116</v>
       </c>
       <c r="D16" s="7">
-        <v>0.4236111111111111</v>
+        <v>0.96527777777777779</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
       </c>
       <c r="F16" s="30">
         <f t="shared" si="0"/>
-        <v>38.000000000000028</v>
+        <v>14.999999999999947</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>119</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B17" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="6">
+        <v>43895</v>
+      </c>
       <c r="C17" s="7">
-        <v>0.43263888888888885</v>
+        <v>0.3972222222222222</v>
       </c>
       <c r="D17" s="7">
-        <v>0.46527777777777773</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
       </c>
       <c r="F17" s="30">
         <f t="shared" si="0"/>
-        <v>46.999999999999993</v>
+        <v>38.000000000000028</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B18" s="6">
-        <v>43896</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B18" s="6"/>
       <c r="C18" s="7">
-        <v>0.37986111111111115</v>
+        <v>0.43263888888888885</v>
       </c>
       <c r="D18" s="7">
-        <v>0.40625</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="E18" s="5">
         <v>0</v>
       </c>
       <c r="F18" s="30">
         <f t="shared" si="0"/>
-        <v>37.999999999999943</v>
+        <v>46.999999999999993</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="I18" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7">
-        <v>0.55763888888888891</v>
+        <v>0.73055555555555562</v>
       </c>
       <c r="D19" s="7">
-        <v>0.56388888888888888</v>
+        <v>0.75347222222222221</v>
       </c>
       <c r="E19" s="5">
         <v>0</v>
       </c>
       <c r="F19" s="30">
         <f t="shared" si="0"/>
-        <v>8.999999999999968</v>
+        <v>32.999999999999886</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B20" s="6">
-        <v>43899</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B20" s="6"/>
       <c r="C20" s="7">
-        <v>0.72430555555555554</v>
+        <v>0.95208333333333339</v>
       </c>
       <c r="D20" s="7">
-        <v>0.74930555555555556</v>
+        <v>0.97499999999999998</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
       </c>
       <c r="F20" s="30">
         <f t="shared" si="0"/>
-        <v>36.000000000000028</v>
+        <v>32.999999999999886</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="6">
+        <v>43896</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="D21" s="7">
+        <v>0.40625</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
       <c r="F21" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+        <v>37.999999999999943</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>122</v>
+      </c>
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="5"/>
+      <c r="C22" s="7">
+        <v>0.55763888888888891</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.56388888888888888</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
+      </c>
       <c r="F22" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+        <v>8.999999999999968</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="14">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
+        <v>17</v>
+      </c>
+      <c r="B23" s="6">
+        <v>43899</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.72430555555555554</v>
+      </c>
+      <c r="D23" s="7">
+        <v>0.74930555555555556</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0</v>
+      </c>
       <c r="F23" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="22"/>
+        <v>36.000000000000028</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="14">
+        <v>18</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.76666666666666661</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0</v>
+      </c>
+      <c r="F24" s="30">
+        <f t="shared" si="0"/>
+        <v>23.999999999999915</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14">
+        <v>19</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14">
+        <v>20</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="22"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="31">
-        <f>SUM(F7:F23)</f>
-        <v>598.00000000000023</v>
-      </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="31">
+        <f>SUM(F7:F26)</f>
+        <v>702.99999999999989</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A27:E27"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>

<commit_message>
VL29 - MeasuresPageModel Index asjade refaktoorimine +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2089ACC-09FD-4B1D-A6C4-16C532E2EE06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCDA5EE-B805-4795-B927-DBBEE8F81562}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7452" yWindow="432" windowWidth="15588" windowHeight="11928" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="139">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -446,6 +446,21 @@
   </si>
   <si>
     <t>VL 28</t>
+  </si>
+  <si>
+    <t>VL29</t>
+  </si>
+  <si>
+    <t>MeasuresPageModel Index asjade refaktoorimine</t>
+  </si>
+  <si>
+    <t>Koodi seletamine</t>
+  </si>
+  <si>
+    <t>VL30</t>
+  </si>
+  <si>
+    <t>BasePageModel lisamine</t>
   </si>
 </sst>
 </file>
@@ -455,7 +470,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,6 +482,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -798,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -999,6 +1020,52 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5126,23 +5193,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11" style="66" customWidth="1"/>
-    <col min="7" max="7" width="55.77734375" customWidth="1"/>
-    <col min="8" max="8" width="63.44140625" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="26.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="91" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="92" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="93" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="93" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="91" customWidth="1"/>
+    <col min="6" max="6" width="11" style="94" customWidth="1"/>
+    <col min="7" max="7" width="55.77734375" style="91" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" style="91" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" style="91" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="91" customWidth="1"/>
+    <col min="11" max="13" width="8.77734375" style="91"/>
+    <col min="14" max="14" width="26.77734375" style="91" customWidth="1"/>
+    <col min="15" max="16384" width="8.77734375" style="91"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -5177,32 +5246,32 @@
         <v>1</v>
       </c>
       <c r="B4" s="87"/>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="97"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="98"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="100"/>
+    </row>
+    <row r="6" spans="1:14" s="101" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="69" t="s">
         <v>3</v>
       </c>
@@ -5233,327 +5302,357 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
+      <c r="A7" s="102">
         <v>1</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="103">
         <v>43900</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="104">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="104">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E7" s="17">
-        <v>0</v>
-      </c>
-      <c r="F7" s="30">
+      <c r="E7" s="105">
+        <v>0</v>
+      </c>
+      <c r="F7" s="106">
         <f>(D7-C7)*1440</f>
         <v>75.000000000000057</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="105" t="s">
         <v>130</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="18"/>
-      <c r="N7" t="s">
+      <c r="I7" s="105"/>
+      <c r="J7" s="107"/>
+      <c r="N7" s="91" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
+      <c r="A8" s="102">
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7">
+      <c r="B8" s="108"/>
+      <c r="C8" s="109">
         <v>0.69861111111111107</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="109">
         <v>0.70277777777777783</v>
       </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="30">
+      <c r="E8" s="110">
+        <v>0</v>
+      </c>
+      <c r="F8" s="106">
         <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
         <v>6.0000000000001386</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="110" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="8"/>
-      <c r="N8" t="s">
+      <c r="I8" s="110"/>
+      <c r="J8" s="111"/>
+      <c r="N8" s="91" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
+      <c r="A9" s="102">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7">
+      <c r="B9" s="108"/>
+      <c r="C9" s="109">
         <v>0.88611111111111107</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="109">
         <v>0.91041666666666676</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="30">
+      <c r="E9" s="110">
+        <v>0</v>
+      </c>
+      <c r="F9" s="106">
         <f t="shared" si="0"/>
         <v>35.000000000000199</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="110" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="8"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="111"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14">
+      <c r="A10" s="102">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="8"/>
+      <c r="B10" s="108">
+        <v>43901</v>
+      </c>
+      <c r="C10" s="109">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D10" s="109">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="E10" s="110">
+        <v>0</v>
+      </c>
+      <c r="F10" s="106">
+        <f t="shared" si="0"/>
+        <v>85.000000000000014</v>
+      </c>
+      <c r="G10" s="110" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="110" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="110"/>
+      <c r="J10" s="111"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14">
+      <c r="A11" s="102">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="8"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="109">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="D11" s="109">
+        <v>0.45</v>
+      </c>
+      <c r="E11" s="110">
+        <v>0</v>
+      </c>
+      <c r="F11" s="106">
+        <f t="shared" si="0"/>
+        <v>83.000000000000028</v>
+      </c>
+      <c r="G11" s="110" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="112" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="110" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="111"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
+      <c r="A12" s="102">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="8"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="110" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="110" t="s">
+        <v>138</v>
+      </c>
+      <c r="I12" s="110"/>
+      <c r="J12" s="111"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14">
+      <c r="A13" s="102">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="8"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="111"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14">
+      <c r="A14" s="102">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="8"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="109"/>
+      <c r="D14" s="109"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="110"/>
+      <c r="H14" s="110"/>
+      <c r="I14" s="110"/>
+      <c r="J14" s="111"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
+      <c r="A15" s="102">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="8"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="109"/>
+      <c r="D15" s="109"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="110"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="111"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
+      <c r="A16" s="102">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="8"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="109"/>
+      <c r="E16" s="110"/>
+      <c r="F16" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="110"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="110"/>
+      <c r="J16" s="111"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
+      <c r="A17" s="102">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="8"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="109"/>
+      <c r="D17" s="109"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="110"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="111"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14">
+      <c r="A18" s="102">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="8"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="109"/>
+      <c r="D18" s="109"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="110"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
+      <c r="J18" s="111"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14">
+      <c r="A19" s="102">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="8"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="110"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="110"/>
+      <c r="J19" s="111"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14">
+      <c r="A20" s="102">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="8"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="109"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="110"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
+      <c r="J20" s="111"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14">
+      <c r="A21" s="102">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="8"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="110"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="111"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14">
+      <c r="A22" s="102">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="114"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="106">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="116"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="71" t="s">
@@ -5565,12 +5664,12 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>116.0000000000004</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
+        <v>284.00000000000045</v>
+      </c>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5583,7 +5682,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
VL30 - BasePageModel loomine +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCDA5EE-B805-4795-B927-DBBEE8F81562}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6CC87C-2CA8-4668-B30F-D62A3275A71E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7452" yWindow="432" windowWidth="15588" windowHeight="11928" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="140">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>BasePageModel lisamine</t>
+  </si>
+  <si>
+    <t>VL30 jätk</t>
   </si>
 </sst>
 </file>
@@ -5193,8 +5196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5458,12 +5461,18 @@
         <v>6</v>
       </c>
       <c r="B12" s="108"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="110"/>
+      <c r="C12" s="109">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="D12" s="109">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E12" s="110">
+        <v>0</v>
+      </c>
       <c r="F12" s="106">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38.999999999999943</v>
       </c>
       <c r="G12" s="110" t="s">
         <v>137</v>
@@ -5480,16 +5489,26 @@
         <v>7</v>
       </c>
       <c r="B13" s="108"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="110"/>
+      <c r="C13" s="109">
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="D13" s="109">
+        <v>0.5625</v>
+      </c>
+      <c r="E13" s="110">
+        <v>0</v>
+      </c>
       <c r="F13" s="106">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="110"/>
+        <v>57.999999999999957</v>
+      </c>
+      <c r="G13" s="110" t="s">
+        <v>139</v>
+      </c>
       <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
+      <c r="I13" s="110" t="s">
+        <v>14</v>
+      </c>
       <c r="J13" s="111"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5664,7 +5683,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>284.00000000000045</v>
+        <v>381.00000000000034</v>
       </c>
       <c r="G23" s="117"/>
       <c r="H23" s="117"/>

</xml_diff>

<commit_message>
VL31-testide abifunktsioonide lisamine; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6CC87C-2CA8-4668-B30F-D62A3275A71E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0266DD-977E-4AA6-AA63-B7760E54341D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7452" yWindow="432" windowWidth="15588" windowHeight="11928" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="192" windowWidth="15588" windowHeight="11928" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="143">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -464,6 +464,15 @@
   </si>
   <si>
     <t>VL30 jätk</t>
+  </si>
+  <si>
+    <t>VL31</t>
+  </si>
+  <si>
+    <t>VL31 jätk</t>
+  </si>
+  <si>
+    <t>Testide abifunktsioonide lisamine</t>
   </si>
 </sst>
 </file>
@@ -5196,8 +5205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5517,15 +5526,25 @@
         <v>8</v>
       </c>
       <c r="B14" s="108"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="110"/>
+      <c r="C14" s="109">
+        <v>0.76180555555555562</v>
+      </c>
+      <c r="D14" s="109">
+        <v>0.78541666666666676</v>
+      </c>
+      <c r="E14" s="110">
+        <v>0</v>
+      </c>
       <c r="F14" s="106">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
+        <v>34.000000000000043</v>
+      </c>
+      <c r="G14" s="110" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="110" t="s">
+        <v>142</v>
+      </c>
       <c r="I14" s="110"/>
       <c r="J14" s="111"/>
     </row>
@@ -5535,16 +5554,26 @@
         <v>9</v>
       </c>
       <c r="B15" s="108"/>
-      <c r="C15" s="109"/>
-      <c r="D15" s="109"/>
-      <c r="E15" s="110"/>
+      <c r="C15" s="109">
+        <v>0.9277777777777777</v>
+      </c>
+      <c r="D15" s="109">
+        <v>0.94305555555555554</v>
+      </c>
+      <c r="E15" s="110">
+        <v>0</v>
+      </c>
       <c r="F15" s="106">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="110"/>
+        <v>22.000000000000082</v>
+      </c>
+      <c r="G15" s="110" t="s">
+        <v>141</v>
+      </c>
       <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
+      <c r="I15" s="110" t="s">
+        <v>14</v>
+      </c>
       <c r="J15" s="111"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5683,7 +5712,7 @@
       <c r="E23" s="73"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>381.00000000000034</v>
+        <v>437.00000000000045</v>
       </c>
       <c r="G23" s="117"/>
       <c r="H23" s="117"/>

</xml_diff>

<commit_message>
VL32 - testid; IsDataTested annab 2 viga ikkagi; midagi on puudu; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0266DD-977E-4AA6-AA63-B7760E54341D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A787BB-A626-4DE9-8BE3-7FB4E2795D8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="192" windowWidth="15588" windowHeight="11928" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="192" windowWidth="15588" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="149">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -473,6 +473,24 @@
   </si>
   <si>
     <t>Testide abifunktsioonide lisamine</t>
+  </si>
+  <si>
+    <t>IsQuantityTested, IsTested Data alt annab vea</t>
+  </si>
+  <si>
+    <t>VL32 36:31</t>
+  </si>
+  <si>
+    <t>Clean Code raamat</t>
+  </si>
+  <si>
+    <t>VL 32 jätk</t>
+  </si>
+  <si>
+    <t>VL32 jätk</t>
+  </si>
+  <si>
+    <t>IsDataTested annab vea ikkagi!!</t>
   </si>
 </sst>
 </file>
@@ -967,6 +985,34 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1033,10 +1079,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1054,30 +1096,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1416,68 +1434,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="81">
+      <c r="G4" s="103">
         <v>43863</v>
       </c>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1959,13 +1977,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0.71180555555555591</v>
@@ -2015,68 +2033,68 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="81">
+      <c r="G4" s="103">
         <v>43871</v>
       </c>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2664,13 +2682,13 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="73"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="95"/>
       <c r="F27" s="25">
         <f>SUM(F7:F26)</f>
         <v>0.77291666666666681</v>
@@ -2720,66 +2738,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3217,13 +3235,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>1260.0000000000002</v>
@@ -3831,66 +3849,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4483,13 +4501,13 @@
       <c r="J27" s="22"/>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="88" t="s">
+      <c r="A28" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="90"/>
+      <c r="B28" s="111"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="112"/>
       <c r="F28" s="31">
         <f>SUM(F7:F27)</f>
         <v>1058.0000000000002</v>
@@ -4539,66 +4557,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5170,13 +5188,13 @@
       <c r="J26" s="22"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="73"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="94"/>
+      <c r="E27" s="95"/>
       <c r="F27" s="31">
         <f>SUM(F7:F26)</f>
         <v>702.99999999999989</v>
@@ -5203,91 +5221,91 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="91" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="92" customWidth="1"/>
-    <col min="3" max="3" width="6.44140625" style="93" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" style="93" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="91" customWidth="1"/>
-    <col min="6" max="6" width="11" style="94" customWidth="1"/>
-    <col min="7" max="7" width="55.77734375" style="91" customWidth="1"/>
-    <col min="8" max="8" width="63.44140625" style="91" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" style="91" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="91" customWidth="1"/>
-    <col min="11" max="13" width="8.77734375" style="91"/>
-    <col min="14" max="14" width="26.77734375" style="91" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="91"/>
+    <col min="1" max="1" width="3.33203125" style="69" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="70" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="71" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="71" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" style="69" customWidth="1"/>
+    <col min="6" max="6" width="11" style="72" customWidth="1"/>
+    <col min="7" max="7" width="55.77734375" style="69" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" style="69" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" style="69" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="69" customWidth="1"/>
+    <col min="11" max="13" width="8.77734375" style="69"/>
+    <col min="14" max="14" width="26.77734375" style="69" customWidth="1"/>
+    <col min="15" max="16384" width="8.77734375" style="69"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="95" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="115"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="98"/>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="100"/>
-    </row>
-    <row r="6" spans="1:14" s="101" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="A5" s="116"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="117"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="118"/>
+    </row>
+    <row r="6" spans="1:14" s="73" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5314,414 +5332,652 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="102">
+      <c r="A7" s="74">
         <v>1</v>
       </c>
-      <c r="B7" s="103">
+      <c r="B7" s="75">
         <v>43900</v>
       </c>
-      <c r="C7" s="104">
+      <c r="C7" s="76">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D7" s="104">
+      <c r="D7" s="76">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E7" s="105">
-        <v>0</v>
-      </c>
-      <c r="F7" s="106">
+      <c r="E7" s="77">
+        <v>0</v>
+      </c>
+      <c r="F7" s="78">
         <f>(D7-C7)*1440</f>
         <v>75.000000000000057</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="105" t="s">
+      <c r="H7" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="I7" s="105"/>
-      <c r="J7" s="107"/>
-      <c r="N7" s="91" t="s">
+      <c r="I7" s="77"/>
+      <c r="J7" s="79"/>
+      <c r="N7" s="69" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="102">
+      <c r="A8" s="74">
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="109">
+      <c r="B8" s="80"/>
+      <c r="C8" s="81">
         <v>0.69861111111111107</v>
       </c>
-      <c r="D8" s="109">
+      <c r="D8" s="81">
         <v>0.70277777777777783</v>
       </c>
-      <c r="E8" s="110">
-        <v>0</v>
-      </c>
-      <c r="F8" s="106">
-        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+      <c r="E8" s="82">
+        <v>0</v>
+      </c>
+      <c r="F8" s="78">
+        <f t="shared" ref="F8:F32" si="0">(D8-C8)*1440</f>
         <v>6.0000000000001386</v>
       </c>
-      <c r="G8" s="110" t="s">
+      <c r="G8" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="H8" s="110" t="s">
+      <c r="H8" s="82" t="s">
         <v>132</v>
       </c>
-      <c r="I8" s="110"/>
-      <c r="J8" s="111"/>
-      <c r="N8" s="91" t="s">
+      <c r="I8" s="82"/>
+      <c r="J8" s="83"/>
+      <c r="N8" s="69" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="102">
-        <f t="shared" ref="A9:A22" si="1">A8+1</f>
+      <c r="A9" s="74">
+        <f t="shared" ref="A9:A32" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="109">
+      <c r="B9" s="80"/>
+      <c r="C9" s="81">
         <v>0.88611111111111107</v>
       </c>
-      <c r="D9" s="109">
+      <c r="D9" s="81">
         <v>0.91041666666666676</v>
       </c>
-      <c r="E9" s="110">
-        <v>0</v>
-      </c>
-      <c r="F9" s="106">
+      <c r="E9" s="82">
+        <v>0</v>
+      </c>
+      <c r="F9" s="78">
         <f t="shared" si="0"/>
         <v>35.000000000000199</v>
       </c>
-      <c r="G9" s="110" t="s">
+      <c r="G9" s="82" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110" t="s">
+      <c r="H9" s="82"/>
+      <c r="I9" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="111"/>
+      <c r="J9" s="83"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="102">
-        <f t="shared" si="1"/>
+      <c r="A10" s="74">
         <v>4</v>
       </c>
-      <c r="B10" s="108">
+      <c r="B10" s="80">
         <v>43901</v>
       </c>
-      <c r="C10" s="109">
+      <c r="C10" s="81">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D10" s="109">
+      <c r="D10" s="81">
         <v>0.3923611111111111</v>
       </c>
-      <c r="E10" s="110">
-        <v>0</v>
-      </c>
-      <c r="F10" s="106">
+      <c r="E10" s="82">
+        <v>0</v>
+      </c>
+      <c r="F10" s="78">
         <f t="shared" si="0"/>
         <v>85.000000000000014</v>
       </c>
-      <c r="G10" s="110" t="s">
+      <c r="G10" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="110" t="s">
+      <c r="H10" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="I10" s="110"/>
-      <c r="J10" s="111"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="83"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="102">
-        <f t="shared" si="1"/>
+      <c r="A11" s="74">
+        <f t="shared" ref="A11:A32" si="2">A10+1</f>
         <v>5</v>
       </c>
-      <c r="B11" s="108"/>
-      <c r="C11" s="109">
+      <c r="B11" s="80"/>
+      <c r="C11" s="81">
         <v>0.3923611111111111</v>
       </c>
-      <c r="D11" s="109">
+      <c r="D11" s="81">
         <v>0.45</v>
       </c>
-      <c r="E11" s="110">
-        <v>0</v>
-      </c>
-      <c r="F11" s="106">
+      <c r="E11" s="82">
+        <v>0</v>
+      </c>
+      <c r="F11" s="78">
         <f t="shared" si="0"/>
         <v>83.000000000000028</v>
       </c>
-      <c r="G11" s="110" t="s">
+      <c r="G11" s="82" t="s">
         <v>134</v>
       </c>
-      <c r="H11" s="112" t="s">
+      <c r="H11" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="I11" s="110" t="s">
+      <c r="I11" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J11" s="111"/>
+      <c r="J11" s="83"/>
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="102">
+      <c r="A12" s="74">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B12" s="108"/>
-      <c r="C12" s="109">
+      <c r="B12" s="80"/>
+      <c r="C12" s="81">
         <v>0.48333333333333334</v>
       </c>
-      <c r="D12" s="109">
+      <c r="D12" s="81">
         <v>0.51041666666666663</v>
       </c>
-      <c r="E12" s="110">
-        <v>0</v>
-      </c>
-      <c r="F12" s="106">
+      <c r="E12" s="82">
+        <v>0</v>
+      </c>
+      <c r="F12" s="78">
         <f t="shared" si="0"/>
         <v>38.999999999999943</v>
       </c>
-      <c r="G12" s="110" t="s">
+      <c r="G12" s="82" t="s">
         <v>137</v>
       </c>
-      <c r="H12" s="110" t="s">
+      <c r="H12" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="I12" s="110"/>
-      <c r="J12" s="111"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="83"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="102">
-        <f t="shared" si="1"/>
+      <c r="A13" s="74">
         <v>7</v>
       </c>
-      <c r="B13" s="108"/>
-      <c r="C13" s="109">
+      <c r="B13" s="80"/>
+      <c r="C13" s="81">
         <v>0.52222222222222225</v>
       </c>
-      <c r="D13" s="109">
+      <c r="D13" s="81">
         <v>0.5625</v>
       </c>
-      <c r="E13" s="110">
-        <v>0</v>
-      </c>
-      <c r="F13" s="106">
+      <c r="E13" s="82">
+        <v>0</v>
+      </c>
+      <c r="F13" s="78">
         <f t="shared" si="0"/>
         <v>57.999999999999957</v>
       </c>
-      <c r="G13" s="110" t="s">
+      <c r="G13" s="82" t="s">
         <v>139</v>
       </c>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110" t="s">
+      <c r="H13" s="82"/>
+      <c r="I13" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="111"/>
+      <c r="J13" s="83"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="102">
-        <f t="shared" si="1"/>
+      <c r="A14" s="74">
+        <f t="shared" ref="A14:A32" si="3">A13+1</f>
         <v>8</v>
       </c>
-      <c r="B14" s="108"/>
-      <c r="C14" s="109">
+      <c r="B14" s="80"/>
+      <c r="C14" s="81">
         <v>0.76180555555555562</v>
       </c>
-      <c r="D14" s="109">
+      <c r="D14" s="81">
         <v>0.78541666666666676</v>
       </c>
-      <c r="E14" s="110">
-        <v>0</v>
-      </c>
-      <c r="F14" s="106">
+      <c r="E14" s="82">
+        <v>0</v>
+      </c>
+      <c r="F14" s="78">
         <f t="shared" si="0"/>
         <v>34.000000000000043</v>
       </c>
-      <c r="G14" s="110" t="s">
+      <c r="G14" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="H14" s="110" t="s">
+      <c r="H14" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="I14" s="110"/>
-      <c r="J14" s="111"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="83"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="102">
+      <c r="A15" s="74">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B15" s="108"/>
-      <c r="C15" s="109">
+      <c r="B15" s="80"/>
+      <c r="C15" s="81">
         <v>0.9277777777777777</v>
       </c>
-      <c r="D15" s="109">
+      <c r="D15" s="81">
         <v>0.94305555555555554</v>
       </c>
-      <c r="E15" s="110">
-        <v>0</v>
-      </c>
-      <c r="F15" s="106">
+      <c r="E15" s="82">
+        <v>0</v>
+      </c>
+      <c r="F15" s="78">
         <f t="shared" si="0"/>
         <v>22.000000000000082</v>
       </c>
-      <c r="G15" s="110" t="s">
+      <c r="G15" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110" t="s">
+      <c r="H15" s="82"/>
+      <c r="I15" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="111"/>
+      <c r="J15" s="83"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="102">
-        <f t="shared" si="1"/>
+      <c r="A16" s="74">
         <v>10</v>
       </c>
-      <c r="B16" s="108"/>
-      <c r="C16" s="109"/>
-      <c r="D16" s="109"/>
-      <c r="E16" s="110"/>
-      <c r="F16" s="106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="110"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="111"/>
+      <c r="B16" s="80"/>
+      <c r="C16" s="81">
+        <v>0.96111111111111114</v>
+      </c>
+      <c r="D16" s="81">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="E16" s="82">
+        <v>0</v>
+      </c>
+      <c r="F16" s="78">
+        <f t="shared" si="0"/>
+        <v>25.999999999999908</v>
+      </c>
+      <c r="G16" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="83"/>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="102">
-        <f t="shared" si="1"/>
+      <c r="A17" s="74">
+        <f t="shared" ref="A17:A32" si="4">A16+1</f>
         <v>11</v>
       </c>
-      <c r="B17" s="108"/>
-      <c r="C17" s="109"/>
-      <c r="D17" s="109"/>
-      <c r="E17" s="110"/>
-      <c r="F17" s="106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="110"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="111"/>
+      <c r="B17" s="80">
+        <v>43902</v>
+      </c>
+      <c r="C17" s="81">
+        <v>0.40902777777777777</v>
+      </c>
+      <c r="D17" s="81">
+        <v>0.4597222222222222</v>
+      </c>
+      <c r="E17" s="82">
+        <v>0</v>
+      </c>
+      <c r="F17" s="78">
+        <f t="shared" si="0"/>
+        <v>72.999999999999986</v>
+      </c>
+      <c r="G17" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" s="82"/>
+      <c r="J17" s="83"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="102">
+      <c r="A18" s="74">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B18" s="108"/>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109"/>
-      <c r="E18" s="110"/>
-      <c r="F18" s="106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="111"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="81">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="D18" s="81">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="E18" s="82">
+        <v>0</v>
+      </c>
+      <c r="F18" s="78">
+        <f t="shared" si="0"/>
+        <v>50.999999999999979</v>
+      </c>
+      <c r="G18" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="83"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="102">
-        <f t="shared" si="1"/>
+      <c r="A19" s="74">
         <v>13</v>
       </c>
-      <c r="B19" s="108"/>
-      <c r="C19" s="109"/>
-      <c r="D19" s="109"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="111"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="81">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="D19" s="81">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="E19" s="82">
+        <v>0</v>
+      </c>
+      <c r="F19" s="78">
+        <f t="shared" si="0"/>
+        <v>55.999999999999957</v>
+      </c>
+      <c r="G19" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="83"/>
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="102">
-        <f t="shared" si="1"/>
+      <c r="A20" s="74">
+        <f t="shared" ref="A20:A32" si="5">A19+1</f>
         <v>14</v>
       </c>
-      <c r="B20" s="108"/>
-      <c r="C20" s="109"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="110"/>
-      <c r="F20" s="106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="111"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="81">
+        <v>0.63611111111111118</v>
+      </c>
+      <c r="D20" s="81">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="E20" s="82">
+        <v>0</v>
+      </c>
+      <c r="F20" s="78">
+        <f t="shared" si="0"/>
+        <v>17.999999999999936</v>
+      </c>
+      <c r="G20" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="83"/>
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="102">
+      <c r="A21" s="74">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B21" s="108"/>
-      <c r="C21" s="109"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="110"/>
-      <c r="F21" s="106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="111"/>
+      <c r="B21" s="80">
+        <v>43903</v>
+      </c>
+      <c r="C21" s="81">
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="D21" s="81">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="E21" s="82">
+        <v>0</v>
+      </c>
+      <c r="F21" s="78">
+        <f t="shared" si="0"/>
+        <v>92.000000000000071</v>
+      </c>
+      <c r="G21" s="82" t="s">
+        <v>146</v>
+      </c>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="83"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="102">
-        <f t="shared" si="1"/>
+      <c r="A22" s="74">
         <v>16</v>
       </c>
-      <c r="B22" s="113"/>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="106">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="115"/>
-      <c r="H22" s="115"/>
-      <c r="I22" s="115"/>
-      <c r="J22" s="116"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="81">
+        <v>0.55625000000000002</v>
+      </c>
+      <c r="D22" s="81">
+        <v>0.5708333333333333</v>
+      </c>
+      <c r="E22" s="82">
+        <v>0</v>
+      </c>
+      <c r="F22" s="78">
+        <f t="shared" si="0"/>
+        <v>20.999999999999925</v>
+      </c>
+      <c r="G22" s="82" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="82" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" s="82" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="83"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="74">
+        <f t="shared" ref="A23:A32" si="6">A22+1</f>
+        <v>17</v>
+      </c>
+      <c r="B23" s="80"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="82"/>
+      <c r="H23" s="82"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="83"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="74">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B24" s="80"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="83"/>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="74">
+        <v>19</v>
+      </c>
+      <c r="B25" s="80"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="82"/>
+      <c r="F25" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="83"/>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="74">
+        <f t="shared" ref="A26:A32" si="7">A25+1</f>
+        <v>20</v>
+      </c>
+      <c r="B26" s="80"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="83"/>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="74">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B27" s="80"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="83"/>
+    </row>
+    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="74">
+        <v>22</v>
+      </c>
+      <c r="B28" s="80"/>
+      <c r="C28" s="81"/>
+      <c r="D28" s="81"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="83"/>
+    </row>
+    <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="74">
+        <f t="shared" ref="A29:A32" si="8">A28+1</f>
+        <v>23</v>
+      </c>
+      <c r="B29" s="80"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="83"/>
+    </row>
+    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="74">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B30" s="80"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="83"/>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="74">
+        <v>25</v>
+      </c>
+      <c r="B31" s="80"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="83"/>
+    </row>
+    <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="74">
+        <f t="shared" ref="A32" si="9">A31+1</f>
+        <v>26</v>
+      </c>
+      <c r="B32" s="85"/>
+      <c r="C32" s="86"/>
+      <c r="D32" s="86"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="78">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="87"/>
+      <c r="H32" s="87"/>
+      <c r="I32" s="87"/>
+      <c r="J32" s="88"/>
+    </row>
+    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="31">
-        <f>SUM(F7:F22)</f>
-        <v>437.00000000000045</v>
-      </c>
-      <c r="G23" s="117"/>
-      <c r="H23" s="117"/>
-      <c r="I23" s="117"/>
-      <c r="J23" s="118"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="95"/>
+      <c r="F33" s="31">
+        <f>SUM(F7:F32)</f>
+        <v>774.00000000000023</v>
+      </c>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="89"/>
+      <c r="J33" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A33:E33"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>
@@ -5759,66 +6015,66 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="77"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="80" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="82"/>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="85"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="70"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -6140,13 +6396,13 @@
       <c r="J22" s="22"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="93" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="73"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="95"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>0</v>

</xml_diff>

<commit_message>
VL33 - dropdown lisamine; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A787BB-A626-4DE9-8BE3-7FB4E2795D8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26862E9E-B770-40DE-BA40-8B297F0634E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="192" windowWidth="15588" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72" yWindow="108" windowWidth="16920" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="150">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -491,6 +491,9 @@
   </si>
   <si>
     <t>IsDataTested annab vea ikkagi!!</t>
+  </si>
+  <si>
+    <t>VL33</t>
   </si>
 </sst>
 </file>
@@ -5223,8 +5226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5396,7 +5399,7 @@
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="74">
-        <f t="shared" ref="A9:A32" si="1">A8+1</f>
+        <f t="shared" ref="A9:A30" si="1">A8+1</f>
         <v>3</v>
       </c>
       <c r="B9" s="80"/>
@@ -5453,7 +5456,7 @@
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="74">
-        <f t="shared" ref="A11:A32" si="2">A10+1</f>
+        <f t="shared" ref="A11" si="2">A10+1</f>
         <v>5</v>
       </c>
       <c r="B11" s="80"/>
@@ -5538,7 +5541,7 @@
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="74">
-        <f t="shared" ref="A14:A32" si="3">A13+1</f>
+        <f t="shared" ref="A14" si="3">A13+1</f>
         <v>8</v>
       </c>
       <c r="B14" s="80"/>
@@ -5619,7 +5622,7 @@
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="74">
-        <f t="shared" ref="A17:A32" si="4">A16+1</f>
+        <f t="shared" ref="A17" si="4">A16+1</f>
         <v>11</v>
       </c>
       <c r="B17" s="80">
@@ -5700,7 +5703,7 @@
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="74">
-        <f t="shared" ref="A20:A32" si="5">A19+1</f>
+        <f t="shared" ref="A20" si="5">A19+1</f>
         <v>14</v>
       </c>
       <c r="B20" s="80"/>
@@ -5783,18 +5786,26 @@
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="74">
-        <f t="shared" ref="A23:A32" si="6">A22+1</f>
+        <f t="shared" ref="A23" si="6">A22+1</f>
         <v>17</v>
       </c>
       <c r="B23" s="80"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="82"/>
+      <c r="C23" s="81">
+        <v>0.98263888888888884</v>
+      </c>
+      <c r="D23" s="81">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E23" s="82">
+        <v>0</v>
+      </c>
       <c r="F23" s="78">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="82"/>
+        <v>24.000000000000075</v>
+      </c>
+      <c r="G23" s="82" t="s">
+        <v>149</v>
+      </c>
       <c r="H23" s="82"/>
       <c r="I23" s="82"/>
       <c r="J23" s="83"/>
@@ -5805,16 +5816,26 @@
         <v>18</v>
       </c>
       <c r="B24" s="80"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="82"/>
+      <c r="C24" s="81">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D24" s="81">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="E24" s="82">
+        <v>0</v>
+      </c>
       <c r="F24" s="78">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="82"/>
+        <v>27</v>
+      </c>
+      <c r="G24" s="82" t="s">
+        <v>149</v>
+      </c>
       <c r="H24" s="82"/>
-      <c r="I24" s="82"/>
+      <c r="I24" s="82" t="s">
+        <v>14</v>
+      </c>
       <c r="J24" s="83"/>
     </row>
     <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5836,7 +5857,7 @@
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="74">
-        <f t="shared" ref="A26:A32" si="7">A25+1</f>
+        <f t="shared" ref="A26" si="7">A25+1</f>
         <v>20</v>
       </c>
       <c r="B26" s="80"/>
@@ -5889,7 +5910,7 @@
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="74">
-        <f t="shared" ref="A29:A32" si="8">A28+1</f>
+        <f t="shared" ref="A29" si="8">A28+1</f>
         <v>23</v>
       </c>
       <c r="B29" s="80"/>
@@ -5968,7 +5989,7 @@
       <c r="E33" s="95"/>
       <c r="F33" s="31">
         <f>SUM(F7:F32)</f>
-        <v>774.00000000000023</v>
+        <v>825.00000000000034</v>
       </c>
       <c r="G33" s="89"/>
       <c r="H33" s="89"/>

</xml_diff>

<commit_message>
VL 34-võõrvõtme sisu näitamine; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26862E9E-B770-40DE-BA40-8B297F0634E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC006F4-CFB0-4346-AB1E-0A566D285933}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="72" yWindow="108" windowWidth="16920" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="152">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -494,6 +494,12 @@
   </si>
   <si>
     <t>VL33</t>
+  </si>
+  <si>
+    <t>VL 34</t>
+  </si>
+  <si>
+    <t>Võõrvõtme sisu näitamine</t>
   </si>
 </sst>
 </file>
@@ -5226,8 +5232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5842,17 +5848,31 @@
       <c r="A25" s="74">
         <v>19</v>
       </c>
-      <c r="B25" s="80"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="82"/>
+      <c r="B25" s="80">
+        <v>43904</v>
+      </c>
+      <c r="C25" s="81">
+        <v>0.8027777777777777</v>
+      </c>
+      <c r="D25" s="81">
+        <v>0.84444444444444444</v>
+      </c>
+      <c r="E25" s="82">
+        <v>0</v>
+      </c>
       <c r="F25" s="78">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
+        <v>60.000000000000107</v>
+      </c>
+      <c r="G25" s="82" t="s">
+        <v>150</v>
+      </c>
+      <c r="H25" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" s="82" t="s">
+        <v>14</v>
+      </c>
       <c r="J25" s="83"/>
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5989,7 +6009,7 @@
       <c r="E33" s="95"/>
       <c r="F33" s="31">
         <f>SUM(F7:F32)</f>
-        <v>825.00000000000034</v>
+        <v>885.00000000000045</v>
       </c>
       <c r="G33" s="89"/>
       <c r="H33" s="89"/>

</xml_diff>

<commit_message>
VL 35 - master-detail seose loomine; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC006F4-CFB0-4346-AB1E-0A566D285933}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAAB086-5616-4E2E-8E3C-2C1D337028B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72" yWindow="108" windowWidth="16920" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4656" yWindow="84" windowWidth="16920" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="154">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -500,6 +500,12 @@
   </si>
   <si>
     <t>Võõrvõtme sisu näitamine</t>
+  </si>
+  <si>
+    <t>VL 35</t>
+  </si>
+  <si>
+    <t>Master-Detail seos</t>
   </si>
 </sst>
 </file>
@@ -5233,7 +5239,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5880,17 +5886,31 @@
         <f t="shared" ref="A26" si="7">A25+1</f>
         <v>20</v>
       </c>
-      <c r="B26" s="80"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="82"/>
+      <c r="B26" s="80">
+        <v>43905</v>
+      </c>
+      <c r="C26" s="81">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="D26" s="81">
+        <v>0.58958333333333335</v>
+      </c>
+      <c r="E26" s="82">
+        <v>0</v>
+      </c>
       <c r="F26" s="78">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="82"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="82"/>
+        <v>59.000000000000114</v>
+      </c>
+      <c r="G26" s="82" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" s="82" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="82" t="s">
+        <v>14</v>
+      </c>
       <c r="J26" s="83"/>
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6009,7 +6029,7 @@
       <c r="E33" s="95"/>
       <c r="F33" s="31">
         <f>SUM(F7:F32)</f>
-        <v>885.00000000000045</v>
+        <v>944.00000000000057</v>
       </c>
       <c r="G33" s="89"/>
       <c r="H33" s="89"/>

</xml_diff>

<commit_message>
VL 36 - Master-Detail tööle; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEAAB086-5616-4E2E-8E3C-2C1D337028B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B06710-15A8-44F2-8FD8-BA400D289837}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4656" yWindow="84" windowWidth="16920" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5004" yWindow="432" windowWidth="16920" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="156">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -506,6 +506,12 @@
   </si>
   <si>
     <t>Master-Detail seos</t>
+  </si>
+  <si>
+    <t>VL 36</t>
+  </si>
+  <si>
+    <t>Master-Detail tööle</t>
   </si>
 </sst>
 </file>
@@ -5238,8 +5244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5919,16 +5925,28 @@
         <v>21</v>
       </c>
       <c r="B27" s="80"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="82"/>
+      <c r="C27" s="81">
+        <v>0.74583333333333324</v>
+      </c>
+      <c r="D27" s="81">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="E27" s="82">
+        <v>0</v>
+      </c>
       <c r="F27" s="78">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="82"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="82"/>
+        <v>95.000000000000142</v>
+      </c>
+      <c r="G27" s="82" t="s">
+        <v>154</v>
+      </c>
+      <c r="H27" s="82" t="s">
+        <v>155</v>
+      </c>
+      <c r="I27" s="82" t="s">
+        <v>14</v>
+      </c>
       <c r="J27" s="83"/>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6029,7 +6047,7 @@
       <c r="E33" s="95"/>
       <c r="F33" s="31">
         <f>SUM(F7:F32)</f>
-        <v>944.00000000000057</v>
+        <v>1039.0000000000007</v>
       </c>
       <c r="G33" s="89"/>
       <c r="H33" s="89"/>

</xml_diff>

<commit_message>
VL 37 - master-detail; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B06710-15A8-44F2-8FD8-BA400D289837}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C007B45-267F-48C7-983A-25E668232FD7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5004" yWindow="432" windowWidth="16920" windowHeight="11928" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Nädal5" sheetId="7" r:id="rId5"/>
     <sheet name="Nädal6" sheetId="8" r:id="rId6"/>
     <sheet name="Nädal7" sheetId="10" r:id="rId7"/>
-    <sheet name="Nädal" sheetId="4" r:id="rId8"/>
+    <sheet name="Nädal8" sheetId="11" r:id="rId8"/>
+    <sheet name="Nädal" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="158">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -512,6 +513,12 @@
   </si>
   <si>
     <t>Master-Detail tööle</t>
+  </si>
+  <si>
+    <t>VL 37</t>
+  </si>
+  <si>
+    <t>Master-Detail lõpetamine</t>
   </si>
 </sst>
 </file>
@@ -5244,8 +5251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView showGridLines="0" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6070,11 +6077,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABB2016-151C-42A0-9FC7-01CF9EE19385}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:J23"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6183,6 +6190,453 @@
       <c r="A7" s="14">
         <v>1</v>
       </c>
+      <c r="B7" s="15">
+        <v>43907</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.84166666666666667</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
+        <f>(D7-C7)*1440</f>
+        <v>88</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14">
+        <f>A7+1</f>
+        <v>2</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="30">
+        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="8"/>
+      <c r="N8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14">
+        <f t="shared" ref="A9:A22" si="1">A8+1</f>
+        <v>3</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="14">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="14">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="14">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="93" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="31">
+        <f>SUM(F7:F22)</f>
+        <v>88</v>
+      </c>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="C2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11" style="66" customWidth="1"/>
+    <col min="7" max="7" width="55.77734375" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="96" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="97"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="98"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="101"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="108" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="109"/>
+      <c r="C4" s="102" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="103"/>
+      <c r="H4" s="103"/>
+      <c r="I4" s="103"/>
+      <c r="J4" s="104"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="105"/>
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="107"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="92"/>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>

</xml_diff>

<commit_message>
VL38 - master-detail refaktoorimine + testid; +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C007B45-267F-48C7-983A-25E668232FD7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DDD8FE-019D-4397-85CA-426E4F81AFAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="432" windowWidth="16920" windowHeight="11928" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -37,15 +37,12 @@
         <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="162">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -519,6 +516,18 @@
   </si>
   <si>
     <t>Master-Detail lõpetamine</t>
+  </si>
+  <si>
+    <t>VL38</t>
+  </si>
+  <si>
+    <t>Master-detail refaktoorimine</t>
+  </si>
+  <si>
+    <t>VL38 jätk</t>
+  </si>
+  <si>
+    <t>VL38 lõpuni</t>
   </si>
 </sst>
 </file>
@@ -5424,7 +5433,7 @@
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="74">
-        <f t="shared" ref="A9:A30" si="1">A8+1</f>
+        <f>A8+1</f>
         <v>3</v>
       </c>
       <c r="B9" s="80"/>
@@ -5481,7 +5490,7 @@
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="74">
-        <f t="shared" ref="A11" si="2">A10+1</f>
+        <f>A10+1</f>
         <v>5</v>
       </c>
       <c r="B11" s="80"/>
@@ -5511,7 +5520,7 @@
     </row>
     <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="74">
-        <f t="shared" si="1"/>
+        <f>A11+1</f>
         <v>6</v>
       </c>
       <c r="B12" s="80"/>
@@ -5566,7 +5575,7 @@
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="74">
-        <f t="shared" ref="A14" si="3">A13+1</f>
+        <f>A13+1</f>
         <v>8</v>
       </c>
       <c r="B14" s="80"/>
@@ -5594,7 +5603,7 @@
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="74">
-        <f t="shared" si="1"/>
+        <f>A14+1</f>
         <v>9</v>
       </c>
       <c r="B15" s="80"/>
@@ -5647,7 +5656,7 @@
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="74">
-        <f t="shared" ref="A17" si="4">A16+1</f>
+        <f>A16+1</f>
         <v>11</v>
       </c>
       <c r="B17" s="80">
@@ -5677,7 +5686,7 @@
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="74">
-        <f t="shared" si="1"/>
+        <f>A17+1</f>
         <v>12</v>
       </c>
       <c r="B18" s="80"/>
@@ -5728,7 +5737,7 @@
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="74">
-        <f t="shared" ref="A20" si="5">A19+1</f>
+        <f>A19+1</f>
         <v>14</v>
       </c>
       <c r="B20" s="80"/>
@@ -5754,7 +5763,7 @@
     </row>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="74">
-        <f t="shared" si="1"/>
+        <f>A20+1</f>
         <v>15</v>
       </c>
       <c r="B21" s="80">
@@ -5811,7 +5820,7 @@
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="74">
-        <f t="shared" ref="A23" si="6">A22+1</f>
+        <f>A22+1</f>
         <v>17</v>
       </c>
       <c r="B23" s="80"/>
@@ -5837,7 +5846,7 @@
     </row>
     <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="74">
-        <f t="shared" si="1"/>
+        <f>A23+1</f>
         <v>18</v>
       </c>
       <c r="B24" s="80"/>
@@ -5896,7 +5905,7 @@
     </row>
     <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="74">
-        <f t="shared" ref="A26" si="7">A25+1</f>
+        <f>A25+1</f>
         <v>20</v>
       </c>
       <c r="B26" s="80">
@@ -5928,7 +5937,7 @@
     </row>
     <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="74">
-        <f t="shared" si="1"/>
+        <f>A26+1</f>
         <v>21</v>
       </c>
       <c r="B27" s="80"/>
@@ -5975,7 +5984,7 @@
     </row>
     <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="74">
-        <f t="shared" ref="A29" si="8">A28+1</f>
+        <f>A28+1</f>
         <v>23</v>
       </c>
       <c r="B29" s="80"/>
@@ -5993,7 +6002,7 @@
     </row>
     <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="74">
-        <f t="shared" si="1"/>
+        <f>A29+1</f>
         <v>24</v>
       </c>
       <c r="B30" s="80"/>
@@ -6028,7 +6037,7 @@
     </row>
     <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="74">
-        <f t="shared" ref="A32" si="9">A31+1</f>
+        <f>A31+1</f>
         <v>26</v>
       </c>
       <c r="B32" s="85"/>
@@ -6080,8 +6089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABB2016-151C-42A0-9FC7-01CF9EE19385}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6212,7 +6221,9 @@
       <c r="H7" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="J7" s="18"/>
       <c r="N7" t="s">
         <v>12</v>
@@ -6223,16 +6234,28 @@
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="6">
+        <v>43909</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.66111111111111109</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.70694444444444438</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
       <c r="F8" s="30">
         <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+        <v>65.999999999999929</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="8"/>
       <c r="N8" t="s">
@@ -6245,14 +6268,22 @@
         <v>3</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="7">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
       <c r="F9" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>57.999999999999794</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>160</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
@@ -6263,16 +6294,26 @@
         <v>4</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="7">
+        <v>0.85486111111111107</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.89027777777777783</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
       <c r="F10" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>51.000000000000142</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>161</v>
+      </c>
       <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6501,7 +6542,7 @@
       <c r="E23" s="95"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>88</v>
+        <v>262.99999999999989</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL39 - HtmlExtension meetodite testide raamistikud +logi
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DDD8FE-019D-4397-85CA-426E4F81AFAE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21EB213-62B7-4EB1-A010-D7EBF6219DCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="432" windowWidth="16920" windowHeight="11928" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="1164" windowWidth="16920" windowHeight="11928" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Nädal" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="165">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -528,6 +529,15 @@
   </si>
   <si>
     <t>VL38 lõpuni</t>
+  </si>
+  <si>
+    <t>VL39</t>
+  </si>
+  <si>
+    <t>HtmlExtension meetodite testide raamistikud</t>
+  </si>
+  <si>
+    <t>VL39 26:52</t>
   </si>
 </sst>
 </file>
@@ -1448,6 +1458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
@@ -2047,6 +2058,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A10" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
@@ -2752,6 +2764,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F62BA5A2-FB0D-47BA-AB0F-898D6AC5DDD6}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A5" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
@@ -3305,6 +3318,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB595BE-6E2E-4B1E-A535-41207EE689C5}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A6" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
@@ -3863,6 +3877,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C307C89-0D63-449E-B823-E5272ACC697D}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A9" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
@@ -4571,6 +4586,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD61791-7BB1-422F-B003-B0D8AC44CC15}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
@@ -5258,6 +5274,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{736E9EB0-25E4-4A82-A666-E89E8961B088}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
@@ -6087,10 +6104,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABB2016-151C-42A0-9FC7-01CF9EE19385}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6321,16 +6339,28 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="5"/>
+      <c r="B11" s="6">
+        <v>43910</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
       <c r="F11" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+        <v>30.99999999999989</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="84" t="s">
+        <v>163</v>
+      </c>
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
@@ -6340,14 +6370,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="7">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.53125</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
       <c r="F12" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>38.000000000000028</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
@@ -6358,16 +6396,26 @@
         <v>7</v>
       </c>
       <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="7">
+        <v>0.6381944444444444</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.6777777777777777</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
       <c r="F13" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="5"/>
+        <v>56.999999999999957</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6542,7 +6590,7 @@
       <c r="E23" s="95"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>262.99999999999989</v>
+        <v>388.99999999999972</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
@@ -6560,12 +6608,13 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">

</xml_diff>

<commit_message>
VL41 testide raamistik BasePage klassile Pages ei vüta reference'i Aidsile omaks
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966101E7-CCE3-4C23-8E93-9A5A3A761A52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A4110-546F-4712-9262-0D211BD86DEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2100" yWindow="432" windowWidth="16920" windowHeight="11928" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="171">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -543,6 +543,18 @@
   </si>
   <si>
     <t xml:space="preserve">VL40 </t>
+  </si>
+  <si>
+    <t>VL41</t>
+  </si>
+  <si>
+    <t>Testide raamistik BasePage klassile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vigade parandamine </t>
+  </si>
+  <si>
+    <t>Pages ei võta omaks reference'I Aidsile</t>
   </si>
 </sst>
 </file>
@@ -552,7 +564,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +585,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri "/>
+      <charset val="186"/>
     </font>
   </fonts>
   <fills count="2">
@@ -901,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1065,6 +1082,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1149,7 +1167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1471,7 +1489,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -1486,70 +1504,70 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="102" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="103">
+      <c r="G4" s="104">
         <v>43863</v>
       </c>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1575,7 +1593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -1607,7 +1625,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -1638,7 +1656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -1666,7 +1684,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1696,7 +1714,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1724,7 +1742,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1752,7 +1770,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1780,7 +1798,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -1808,7 +1826,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -1836,7 +1854,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -1868,7 +1886,7 @@
       </c>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -1896,7 +1914,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -1926,7 +1944,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -1956,7 +1974,7 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1984,7 +2002,7 @@
       </c>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2012,7 +2030,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -2030,14 +2048,14 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="93" t="s">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="95"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
       <c r="F23" s="25">
         <f>SUM(F7:F22)</f>
         <v>0.71180555555555591</v>
@@ -2071,7 +2089,7 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -2086,70 +2104,70 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="102" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="103">
+      <c r="G4" s="104">
         <v>43871</v>
       </c>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2175,7 +2193,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -2209,7 +2227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -2242,7 +2260,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A21" si="1">A8+1</f>
         <v>3</v>
@@ -2270,7 +2288,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2302,7 +2320,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -2332,7 +2350,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -2362,7 +2380,7 @@
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -2392,7 +2410,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2422,7 +2440,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2452,7 +2470,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2478,7 +2496,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2504,7 +2522,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -2532,7 +2550,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -2560,7 +2578,7 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -2588,7 +2606,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -2614,7 +2632,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14"/>
       <c r="B22" s="26"/>
       <c r="C22" s="27">
@@ -2637,7 +2655,7 @@
       <c r="I22" s="28"/>
       <c r="J22" s="29"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14"/>
       <c r="B23" s="26"/>
       <c r="C23" s="27">
@@ -2660,7 +2678,7 @@
       <c r="I23" s="28"/>
       <c r="J23" s="29"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="14"/>
       <c r="B24" s="26"/>
       <c r="C24" s="27">
@@ -2683,7 +2701,7 @@
       <c r="I24" s="28"/>
       <c r="J24" s="29"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="14"/>
       <c r="B25" s="26">
         <v>43870</v>
@@ -2710,7 +2728,7 @@
       <c r="I25" s="28"/>
       <c r="J25" s="29"/>
     </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="14">
         <f>A21+1</f>
         <v>16</v>
@@ -2736,14 +2754,14 @@
       <c r="I26" s="21"/>
       <c r="J26" s="22"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="93" t="s">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
+      <c r="A27" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="95"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="96"/>
       <c r="F27" s="25">
         <f>SUM(F7:F26)</f>
         <v>0.77291666666666681</v>
@@ -2777,7 +2795,7 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -2792,68 +2810,68 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="102" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -2879,7 +2897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -2909,7 +2927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -2942,7 +2960,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -2970,7 +2988,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -2998,7 +3016,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -3026,7 +3044,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3052,7 +3070,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3082,7 +3100,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3108,7 +3126,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3136,7 +3154,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3164,7 +3182,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -3192,7 +3210,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3218,7 +3236,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3236,7 +3254,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -3254,7 +3272,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -3272,7 +3290,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -3290,14 +3308,14 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="93" t="s">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="95"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>1260.0000000000002</v>
@@ -3331,7 +3349,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -3346,8 +3364,8 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
       <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
@@ -3361,7 +3379,7 @@
       <c r="I2" s="44"/>
       <c r="J2" s="45"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -3373,7 +3391,7 @@
       <c r="I3" s="47"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15" thickBot="1">
       <c r="A4" s="49" t="s">
         <v>1</v>
       </c>
@@ -3391,7 +3409,7 @@
       <c r="I4" s="52"/>
       <c r="J4" s="53"/>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15" thickBot="1">
       <c r="A5" s="54"/>
       <c r="B5" s="55"/>
       <c r="C5" s="55"/>
@@ -3403,7 +3421,7 @@
       <c r="I5" s="55"/>
       <c r="J5" s="56"/>
     </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
       <c r="A6" s="57" t="s">
         <v>3</v>
       </c>
@@ -3433,7 +3451,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -3463,7 +3481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -3494,7 +3512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -3522,7 +3540,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -3550,7 +3568,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -3582,7 +3600,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -3608,7 +3626,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -3640,7 +3658,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -3666,7 +3684,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -3696,7 +3714,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" s="39" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" s="39" customFormat="1" ht="43.8" thickBot="1">
       <c r="A16" s="32">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -3728,7 +3746,7 @@
       </c>
       <c r="J16" s="38"/>
     </row>
-    <row r="17" spans="1:10" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="29.4" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -3758,7 +3776,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -3786,7 +3804,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3804,7 +3822,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -3822,7 +3840,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -3840,7 +3858,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -3858,7 +3876,7 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="40" t="s">
         <v>21</v>
       </c>
@@ -3890,7 +3908,7 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -3905,68 +3923,68 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="102" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -3992,7 +4010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -4022,7 +4040,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -4057,7 +4075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A20" si="1">A8+1</f>
         <v>3</v>
@@ -4085,7 +4103,7 @@
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -4115,7 +4133,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -4145,7 +4163,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -4173,7 +4191,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -4203,7 +4221,7 @@
       </c>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -4231,7 +4249,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -4259,7 +4277,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -4287,7 +4305,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -4315,7 +4333,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -4345,7 +4363,7 @@
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -4375,7 +4393,7 @@
       </c>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -4405,7 +4423,7 @@
       </c>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <v>15</v>
       </c>
@@ -4434,7 +4452,7 @@
       </c>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <v>16</v>
       </c>
@@ -4461,7 +4479,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14">
         <v>17</v>
       </c>
@@ -4490,7 +4508,7 @@
       </c>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="14">
         <v>18</v>
       </c>
@@ -4507,7 +4525,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="14">
         <v>19</v>
       </c>
@@ -4524,7 +4542,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="14">
         <v>20</v>
       </c>
@@ -4541,7 +4559,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
       <c r="A27" s="14">
         <v>21</v>
       </c>
@@ -4558,14 +4576,14 @@
       <c r="I27" s="21"/>
       <c r="J27" s="22"/>
     </row>
-    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="110" t="s">
+    <row r="28" spans="1:10" ht="15" thickBot="1">
+      <c r="A28" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="111"/>
-      <c r="C28" s="111"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="112"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="113"/>
       <c r="F28" s="31">
         <f>SUM(F7:F27)</f>
         <v>1058.0000000000002</v>
@@ -4599,7 +4617,7 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -4614,68 +4632,68 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="102" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -4701,7 +4719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -4735,7 +4753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <v>2</v>
       </c>
@@ -4767,7 +4785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <v>3</v>
       </c>
@@ -4794,7 +4812,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <v>4</v>
       </c>
@@ -4822,7 +4840,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <v>5</v>
       </c>
@@ -4851,7 +4869,7 @@
       </c>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <v>6</v>
       </c>
@@ -4882,7 +4900,7 @@
       </c>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <v>7</v>
       </c>
@@ -4909,7 +4927,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <v>8</v>
       </c>
@@ -4934,7 +4952,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <v>9</v>
       </c>
@@ -4961,7 +4979,7 @@
       </c>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <v>10</v>
       </c>
@@ -4986,7 +5004,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <v>11</v>
       </c>
@@ -5015,7 +5033,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <v>12</v>
       </c>
@@ -5044,7 +5062,7 @@
       </c>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <v>13</v>
       </c>
@@ -5069,7 +5087,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <v>14</v>
       </c>
@@ -5094,7 +5112,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <v>15</v>
       </c>
@@ -5123,7 +5141,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <v>16</v>
       </c>
@@ -5152,7 +5170,7 @@
       </c>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14">
         <v>17</v>
       </c>
@@ -5183,7 +5201,7 @@
       </c>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="14">
         <v>18</v>
       </c>
@@ -5212,7 +5230,7 @@
       </c>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="14">
         <v>19</v>
       </c>
@@ -5229,7 +5247,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="14">
         <v>20</v>
       </c>
@@ -5246,14 +5264,14 @@
       <c r="I26" s="21"/>
       <c r="J26" s="22"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="93" t="s">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
+      <c r="A27" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
-      <c r="E27" s="95"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="96"/>
       <c r="F27" s="31">
         <f>SUM(F7:F26)</f>
         <v>702.99999999999989</v>
@@ -5287,7 +5305,7 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" style="69" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="70" customWidth="1"/>
@@ -5304,68 +5322,68 @@
     <col min="15" max="16384" width="8.77734375" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="113" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="114" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="113"/>
-      <c r="E4" s="113"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="114"/>
-      <c r="H4" s="114"/>
-      <c r="I4" s="114"/>
-      <c r="J4" s="115"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="116"/>
-      <c r="B5" s="117"/>
-      <c r="C5" s="117"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
-      <c r="J5" s="118"/>
-    </row>
-    <row r="6" spans="1:14" s="73" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="116"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="117"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="119"/>
+    </row>
+    <row r="6" spans="1:14" s="73" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -5391,7 +5409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="74">
         <v>1</v>
       </c>
@@ -5423,7 +5441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="74">
         <f>A7+1</f>
         <v>2</v>
@@ -5454,7 +5472,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="74">
         <f>A8+1</f>
         <v>3</v>
@@ -5482,7 +5500,7 @@
       </c>
       <c r="J9" s="83"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="74">
         <v>4</v>
       </c>
@@ -5511,7 +5529,7 @@
       <c r="I10" s="82"/>
       <c r="J10" s="83"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="74">
         <f>A10+1</f>
         <v>5</v>
@@ -5541,7 +5559,7 @@
       </c>
       <c r="J11" s="83"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="74">
         <f>A11+1</f>
         <v>6</v>
@@ -5569,7 +5587,7 @@
       <c r="I12" s="82"/>
       <c r="J12" s="83"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="74">
         <v>7</v>
       </c>
@@ -5596,7 +5614,7 @@
       </c>
       <c r="J13" s="83"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="74">
         <f>A13+1</f>
         <v>8</v>
@@ -5624,7 +5642,7 @@
       <c r="I14" s="82"/>
       <c r="J14" s="83"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="74">
         <f>A14+1</f>
         <v>9</v>
@@ -5652,7 +5670,7 @@
       </c>
       <c r="J15" s="83"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="74">
         <v>10</v>
       </c>
@@ -5677,7 +5695,7 @@
       <c r="I16" s="82"/>
       <c r="J16" s="83"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="74">
         <f>A16+1</f>
         <v>11</v>
@@ -5707,7 +5725,7 @@
       <c r="I17" s="82"/>
       <c r="J17" s="83"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="74">
         <f>A17+1</f>
         <v>12</v>
@@ -5733,7 +5751,7 @@
       <c r="I18" s="82"/>
       <c r="J18" s="83"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="74">
         <v>13</v>
       </c>
@@ -5758,7 +5776,7 @@
       <c r="I19" s="82"/>
       <c r="J19" s="83"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="74">
         <f>A19+1</f>
         <v>14</v>
@@ -5784,7 +5802,7 @@
       <c r="I20" s="82"/>
       <c r="J20" s="83"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="74">
         <f>A20+1</f>
         <v>15</v>
@@ -5812,7 +5830,7 @@
       <c r="I21" s="82"/>
       <c r="J21" s="83"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="74">
         <v>16</v>
       </c>
@@ -5841,7 +5859,7 @@
       </c>
       <c r="J22" s="83"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="74">
         <f>A22+1</f>
         <v>17</v>
@@ -5867,7 +5885,7 @@
       <c r="I23" s="82"/>
       <c r="J23" s="83"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
       <c r="A24" s="74">
         <f>A23+1</f>
         <v>18</v>
@@ -5895,7 +5913,7 @@
       </c>
       <c r="J24" s="83"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15" thickBot="1">
       <c r="A25" s="74">
         <v>19</v>
       </c>
@@ -5926,7 +5944,7 @@
       </c>
       <c r="J25" s="83"/>
     </row>
-    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="74">
         <f>A25+1</f>
         <v>20</v>
@@ -5958,7 +5976,7 @@
       </c>
       <c r="J26" s="83"/>
     </row>
-    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="15" thickBot="1">
       <c r="A27" s="74">
         <f>A26+1</f>
         <v>21</v>
@@ -5988,7 +6006,7 @@
       </c>
       <c r="J27" s="83"/>
     </row>
-    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15" thickBot="1">
       <c r="A28" s="74">
         <v>22</v>
       </c>
@@ -6005,7 +6023,7 @@
       <c r="I28" s="82"/>
       <c r="J28" s="83"/>
     </row>
-    <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="15" thickBot="1">
       <c r="A29" s="74">
         <f>A28+1</f>
         <v>23</v>
@@ -6023,7 +6041,7 @@
       <c r="I29" s="82"/>
       <c r="J29" s="83"/>
     </row>
-    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15" thickBot="1">
       <c r="A30" s="74">
         <f>A29+1</f>
         <v>24</v>
@@ -6041,7 +6059,7 @@
       <c r="I30" s="82"/>
       <c r="J30" s="83"/>
     </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="15" thickBot="1">
       <c r="A31" s="74">
         <v>25</v>
       </c>
@@ -6058,7 +6076,7 @@
       <c r="I31" s="82"/>
       <c r="J31" s="83"/>
     </row>
-    <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="15" thickBot="1">
       <c r="A32" s="74">
         <f>A31+1</f>
         <v>26</v>
@@ -6076,14 +6094,14 @@
       <c r="I32" s="87"/>
       <c r="J32" s="88"/>
     </row>
-    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="93" t="s">
+    <row r="33" spans="1:10" ht="15" thickBot="1">
+      <c r="A33" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="94"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="95"/>
+      <c r="B33" s="95"/>
+      <c r="C33" s="95"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="96"/>
       <c r="F33" s="31">
         <f>SUM(F7:F32)</f>
         <v>1039.0000000000007</v>
@@ -6114,10 +6132,10 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="93" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -6132,68 +6150,68 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="102" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -6219,7 +6237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -6253,7 +6271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -6286,7 +6304,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A23" si="1">A8+1</f>
         <v>3</v>
@@ -6312,7 +6330,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -6340,7 +6358,7 @@
       </c>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7">
@@ -6359,11 +6377,11 @@
       <c r="G11" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="H11" s="119"/>
+      <c r="H11" s="91"/>
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f>A10+1</f>
         <v>5</v>
@@ -6393,7 +6411,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6419,7 +6437,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -6447,7 +6465,7 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -6475,7 +6493,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -6505,43 +6523,65 @@
       </c>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="7">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0.68819444444444444</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
       <c r="F17" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+        <v>43.000000000000007</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" s="120" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
+      <c r="C18" s="7">
+        <v>0.68888888888888899</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.6958333333333333</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
       <c r="F18" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+        <v>9.9999999999998046</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -6559,7 +6599,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -6577,7 +6617,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -6595,7 +6635,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -6613,7 +6653,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
       <c r="A23" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -6631,17 +6671,17 @@
       <c r="I23" s="21"/>
       <c r="J23" s="22"/>
     </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="93" t="s">
+    <row r="24" spans="1:10" ht="15" thickBot="1">
+      <c r="A24" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="B24" s="94"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="95"/>
+      <c r="B24" s="95"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="96"/>
       <c r="F24" s="31">
         <f>SUM(F7:F23)</f>
-        <v>531.99999999999955</v>
+        <v>584.99999999999932</v>
       </c>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
@@ -6672,7 +6712,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
@@ -6687,68 +6727,68 @@
     <col min="14" max="14" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="98"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="101"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="108" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="99"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="100"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="102"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="109"/>
-      <c r="C4" s="102" t="s">
+      <c r="B4" s="110"/>
+      <c r="C4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="103"/>
       <c r="F4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="103"/>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
-      <c r="J4" s="104"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="105"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
-      <c r="G5" s="106"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="106"/>
-      <c r="J5" s="107"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="91" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="105"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="106"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="107"/>
+      <c r="D5" s="107"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="108"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="92"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
@@ -6774,7 +6814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" ht="15" thickBot="1">
       <c r="A7" s="14">
         <v>1</v>
       </c>
@@ -6796,7 +6836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" ht="15" thickBot="1">
       <c r="A8" s="14">
         <f>A7+1</f>
         <v>2</v>
@@ -6817,7 +6857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
@@ -6835,7 +6875,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" ht="15" thickBot="1">
       <c r="A10" s="14">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -6853,7 +6893,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="15" thickBot="1">
       <c r="A11" s="14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -6871,7 +6911,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15" thickBot="1">
       <c r="A12" s="14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6889,7 +6929,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="15" thickBot="1">
       <c r="A13" s="14">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -6907,7 +6947,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1">
       <c r="A14" s="14">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -6925,7 +6965,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -6943,7 +6983,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -6961,7 +7001,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -6979,7 +7019,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -6997,7 +7037,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -7015,7 +7055,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -7033,7 +7073,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -7051,7 +7091,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -7069,14 +7109,14 @@
       <c r="I22" s="21"/>
       <c r="J22" s="22"/>
     </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="93" t="s">
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="95"/>
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
         <v>0</v>

</xml_diff>

<commit_message>
VL45- Quantity Data Model
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82E15C0-F72F-429A-BB83-62B9EABBAF38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE202411-6A5B-4EF7-A4CD-A717DC75FFA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2796" yWindow="432" windowWidth="16920" windowHeight="11928" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2796" yWindow="432" windowWidth="16920" windowHeight="11928" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nädal 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Nädal6" sheetId="8" r:id="rId6"/>
     <sheet name="Nädal7" sheetId="10" r:id="rId7"/>
     <sheet name="Nädal8" sheetId="11" r:id="rId8"/>
-    <sheet name="Nädal" sheetId="4" r:id="rId9"/>
+    <sheet name="Nädal9" sheetId="12" r:id="rId9"/>
+    <sheet name="Nädal" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="179">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -573,6 +574,12 @@
   </si>
   <si>
     <t>Clean Code konspekt</t>
+  </si>
+  <si>
+    <t>VL45</t>
+  </si>
+  <si>
+    <t>Quantity Data Model</t>
   </si>
 </sst>
 </file>
@@ -2098,6 +2105,444 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet9"/>
+  <dimension ref="A1:N23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="C2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11" style="66" customWidth="1"/>
+    <col min="7" max="7" width="55.77734375" customWidth="1"/>
+    <col min="8" max="8" width="63.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="26.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15" thickBot="1"/>
+    <row r="2" spans="1:14">
+      <c r="A2" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="100"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="101"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="103"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" thickBot="1">
+      <c r="A4" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="111"/>
+      <c r="C4" s="104" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="106"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" thickBot="1">
+      <c r="A5" s="107"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="109"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="29.4" thickBot="1">
+      <c r="A6" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="94"/>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="15" thickBot="1">
+      <c r="A7" s="14">
+        <v>1</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
+        <f>(D7-C7)*1440</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="N7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="15" thickBot="1">
+      <c r="A8" s="14">
+        <f>A7+1</f>
+        <v>2</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="30">
+        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="8"/>
+      <c r="N8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" thickBot="1">
+      <c r="A9" s="14">
+        <f t="shared" ref="A9:A22" si="1">A8+1</f>
+        <v>3</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" ht="15" thickBot="1">
+      <c r="A10" s="14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" ht="15" thickBot="1">
+      <c r="A11" s="14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" ht="15" thickBot="1">
+      <c r="A12" s="14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" ht="15" thickBot="1">
+      <c r="A13" s="14">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:14" ht="15" thickBot="1">
+      <c r="A14" s="14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:14" ht="15" thickBot="1">
+      <c r="A15" s="14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1">
+      <c r="A16" s="14">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1">
+      <c r="A17" s="14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1">
+      <c r="A18" s="14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1">
+      <c r="A19" s="14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1">
+      <c r="A20" s="14">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1">
+      <c r="A21" s="14">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1">
+      <c r="A22" s="14">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="31">
+        <f>SUM(F7:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
@@ -6149,7 +6594,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="93" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="93" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -6818,12 +7263,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0979A2CD-0C4F-4F3F-AF21-9859F6F56A6C}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C2" zoomScale="116" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -6932,18 +7376,28 @@
       <c r="A7" s="14">
         <v>1</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="15">
+        <v>43916</v>
+      </c>
+      <c r="C7" s="16">
+        <v>0.48472222222222222</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0.50763888888888886</v>
+      </c>
       <c r="E7" s="17">
         <v>0</v>
       </c>
       <c r="F7" s="30">
         <f>(D7-C7)*1440</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
+        <v>32.999999999999964</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
       <c r="N7" t="s">
@@ -7233,7 +7687,7 @@
       <c r="E23" s="97"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>0</v>
+        <v>32.999999999999964</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL46A Quantity Data Tests
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE202411-6A5B-4EF7-A4CD-A717DC75FFA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25A5C12-994C-4BBB-8F6A-7353BD4E7306}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2796" yWindow="432" windowWidth="16920" windowHeight="11928" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="181">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -580,6 +580,12 @@
   </si>
   <si>
     <t>Quantity Data Model</t>
+  </si>
+  <si>
+    <t>Quantity Data Tests, +Pages testis viga korda</t>
+  </si>
+  <si>
+    <t>VL46A</t>
   </si>
 </sst>
 </file>
@@ -7266,8 +7272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0979A2CD-0C4F-4F3F-AF21-9859F6F56A6C}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -7398,7 +7404,9 @@
       <c r="H7" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="I7" s="17"/>
+      <c r="I7" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="J7" s="18"/>
       <c r="N7" t="s">
         <v>12</v>
@@ -7410,16 +7418,28 @@
         <v>2</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="7">
+        <v>0.94305555555555554</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.96875</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
       <c r="F8" s="30">
         <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+        <v>37.000000000000028</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J8" s="8"/>
       <c r="N8" t="s">
         <v>15</v>
@@ -7687,7 +7707,7 @@
       <c r="E23" s="97"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>32.999999999999964</v>
+        <v>70</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
VL46B - QuantityData Tests korda
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25A5C12-994C-4BBB-8F6A-7353BD4E7306}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB29C013-F55D-4B0E-9F9B-0FFF1DF6977D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2796" yWindow="432" windowWidth="16920" windowHeight="11928" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="183">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t>VL46A</t>
+  </si>
+  <si>
+    <t>VL46B</t>
+  </si>
+  <si>
+    <t>Quantity Data Tests lõpp</t>
   </si>
 </sst>
 </file>
@@ -7272,8 +7278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0979A2CD-0C4F-4F3F-AF21-9859F6F56A6C}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -7450,17 +7456,31 @@
         <f t="shared" ref="A9:A22" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="6">
+        <v>43917</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.40416666666666662</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
       <c r="F9" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+        <v>18.000000000000096</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1">
@@ -7707,7 +7727,7 @@
       <c r="E23" s="97"/>
       <c r="F23" s="31">
         <f>SUM(F7:F22)</f>
-        <v>70</v>
+        <v>88.000000000000099</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>

</xml_diff>

<commit_message>
Aids kaust + delete/edit muudatused
</commit_message>
<xml_diff>
--- a/PROGE_Time recording log.xlsx
+++ b/PROGE_Time recording log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kasutaja\source\repos\AnnabelMa\Kodutood\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70648816-558D-4FF5-8CB5-E906A313D889}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0F71C5-D953-40CD-ABEC-A92427C874E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="432" windowWidth="16920" windowHeight="11928" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="189">
   <si>
     <t>Time recording log:</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>"Kanban Fundamentals"</t>
+  </si>
+  <si>
+    <t>VL47</t>
+  </si>
+  <si>
+    <t>Quantity Domain klassid ja testid</t>
+  </si>
+  <si>
+    <t>Aids kaust korda uuesti + referenced</t>
   </si>
 </sst>
 </file>
@@ -7285,10 +7294,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0979A2CD-0C4F-4F3F-AF21-9859F6F56A6C}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="87" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -7443,7 +7452,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="30">
-        <f t="shared" ref="F8:F22" si="0">(D8-C8)*1440</f>
+        <f t="shared" ref="F8:F23" si="0">(D8-C8)*1440</f>
         <v>37.000000000000028</v>
       </c>
       <c r="G8" s="5" t="s">
@@ -7462,7 +7471,7 @@
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1">
       <c r="A9" s="14">
-        <f t="shared" ref="A9:A22" si="1">A8+1</f>
+        <f t="shared" ref="A9:A23" si="1">A8+1</f>
         <v>3</v>
       </c>
       <c r="B9" s="6">
@@ -7609,27 +7618,32 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1">
-      <c r="A14" s="14">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
+      <c r="A14" s="14"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="7">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
       <c r="F14" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="5"/>
+        <v>31.999999999999886</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1">
       <c r="A15" s="14">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>A13+1</f>
+        <v>8</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
@@ -7639,15 +7653,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>187</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:14" ht="15" thickBot="1">
       <c r="A16" s="14">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -7665,7 +7683,7 @@
     <row r="17" spans="1:10" ht="15" thickBot="1">
       <c r="A17" s="14">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -7683,7 +7701,7 @@
     <row r="18" spans="1:10" ht="15" thickBot="1">
       <c r="A18" s="14">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
@@ -7701,7 +7719,7 @@
     <row r="19" spans="1:10" ht="15" thickBot="1">
       <c r="A19" s="14">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
@@ -7719,7 +7737,7 @@
     <row r="20" spans="1:10" ht="15" thickBot="1">
       <c r="A20" s="14">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -7737,7 +7755,7 @@
     <row r="21" spans="1:10" ht="15" thickBot="1">
       <c r="A21" s="14">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -7755,41 +7773,59 @@
     <row r="22" spans="1:10" ht="15" thickBot="1">
       <c r="A22" s="14">
         <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1">
+      <c r="A23" s="14">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-    </row>
-    <row r="23" spans="1:10" ht="15" thickBot="1">
-      <c r="A23" s="95" t="s">
+      <c r="B23" s="19"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1">
+      <c r="A24" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="31">
-        <f>SUM(F7:F22)</f>
-        <v>204.00000000000014</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="97"/>
+      <c r="F24" s="31">
+        <f>SUM(F7:F23)</f>
+        <v>236.00000000000003</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A2:J3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:E4"/>

</xml_diff>